<commit_message>
continued the rest of the columns
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\lending_club_credit_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D008EF1-D0F9-46B7-85F5-FE036950A726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AB2085-5B9A-4364-94BB-E0D8B533CAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="314">
   <si>
     <t>Column Name</t>
   </si>
@@ -985,12 +985,84 @@
   <si>
     <t>7.5% missing -&gt; replace to be unknown</t>
   </si>
+  <si>
+    <t>Text handling (All upper or all lower, check 1-length, etc)</t>
+  </si>
+  <si>
+    <t>Unify (ANY &amp; OTHER &amp; NONE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review outliers </t>
+  </si>
+  <si>
+    <t>Was income verified by LendingClub?</t>
+  </si>
+  <si>
+    <t>Unify(Verfied, Source verfied) and unify characters</t>
+  </si>
+  <si>
+    <t>Date (YYYY-MM)</t>
+  </si>
+  <si>
+    <t>When the load funded</t>
+  </si>
+  <si>
+    <t>Convert format to YYYY-MM</t>
+  </si>
+  <si>
+    <t>current status of the loan</t>
+  </si>
+  <si>
+    <t>Cleansing the outlier values having no meaning</t>
+  </si>
+  <si>
+    <t>modified repayment arrangement between the lender and borrower when the borrower is having difficulty making regular payments</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper </t>
+  </si>
+  <si>
+    <t>Loan link on lending club website</t>
+  </si>
+  <si>
+    <t>Drop the column,no analytical value</t>
+  </si>
+  <si>
+    <t>Entred by the borrower shows the reason for the loan</t>
+  </si>
+  <si>
+    <t>one_to_one</t>
+  </si>
+  <si>
+    <t>Drop the column, redundant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same as purpose </t>
+  </si>
+  <si>
+    <t>location provided by the borrower</t>
+  </si>
+  <si>
+    <t>The borrower’s  monthly debt payments excluding mortgage and the requested loan, divided by the borrower’s monthly income.</t>
+  </si>
+  <si>
+    <t>exclude negatives, it would be represented as a ratio</t>
+  </si>
+  <si>
+    <t>Number of 30+ day delinquencies in past 2 years</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1138,6 +1210,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1504,7 +1583,7 @@
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1535,20 +1614,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="41"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1929,7 +2007,7 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2041,13 +2119,13 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>152</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -2056,18 +2134,18 @@
       <c r="E6" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>151</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>153</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2076,15 +2154,15 @@
       <c r="E7" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="14" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -2101,7 +2179,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="A9" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2121,13 +2199,13 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>277</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -2136,18 +2214,18 @@
       <c r="E10" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="15" t="s">
         <v>279</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2156,18 +2234,18 @@
       <c r="E11" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="14" t="s">
+      <c r="A12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>281</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2176,18 +2254,18 @@
       <c r="E12" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:6" ht="28.5">
+      <c r="A13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>283</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2196,15 +2274,18 @@
       <c r="E13" s="2" t="s">
         <v>275</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14" t="s">
+      <c r="A14" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="15" t="s">
         <v>284</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -2218,10 +2299,13 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="14" t="s">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>286</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2230,152 +2314,269 @@
       <c r="E15" s="2" t="s">
         <v>275</v>
       </c>
+      <c r="F15" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="14" t="s">
+      <c r="A16" t="s">
         <v>86</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="14" t="s">
+      <c r="F16" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.5">
+      <c r="A17" t="s">
         <v>158</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>293</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="14" t="s">
+      <c r="F17" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>296</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="14" t="s">
+      <c r="F18" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.5">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14" t="s">
+      <c r="F19" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
         <v>159</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C20" t="s">
+        <v>300</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14" t="s">
+      <c r="F20" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
         <v>160</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>303</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="14" t="s">
+      <c r="F21" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
         <v>161</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="14" t="s">
+      <c r="F22" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
         <v>68</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>305</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="14" t="s">
+      <c r="F23" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
         <v>162</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>308</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="14" t="s">
+      <c r="F24" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
         <v>163</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>309</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="14" t="s">
+      <c r="F25" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>91</v>
       </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>309</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="14" t="s">
+      <c r="F26" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.5">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>310</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="14" t="s">
+      <c r="F27" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>112</v>
       </c>
+      <c r="B28" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>312</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="14" t="s">
+      <c r="F28" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
         <v>164</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2385,8 +2586,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2396,8 +2597,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
         <v>101</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2407,8 +2608,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
         <v>165</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2419,7 +2620,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="14" t="s">
+      <c r="A33" t="s">
         <v>166</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2430,7 +2631,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="14" t="s">
+      <c r="A34" t="s">
         <v>167</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2441,7 +2642,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="14" t="s">
+      <c r="A35" t="s">
         <v>107</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2452,7 +2653,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="14" t="s">
+      <c r="A36" t="s">
         <v>115</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2463,7 +2664,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="14" t="s">
+      <c r="A37" t="s">
         <v>168</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2474,7 +2675,7 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="14" t="s">
+      <c r="A38" t="s">
         <v>104</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2485,7 +2686,7 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="14" t="s">
+      <c r="A39" t="s">
         <v>110</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2496,7 +2697,7 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="14" t="s">
+      <c r="A40" t="s">
         <v>169</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2507,7 +2708,7 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="14" t="s">
+      <c r="A41" t="s">
         <v>128</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2518,7 +2719,7 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="14" t="s">
+      <c r="A42" t="s">
         <v>170</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2529,7 +2730,7 @@
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="14" t="s">
+      <c r="A43" t="s">
         <v>117</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2540,7 +2741,7 @@
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="14" t="s">
+      <c r="A44" t="s">
         <v>171</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2551,7 +2752,7 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="14" t="s">
+      <c r="A45" t="s">
         <v>120</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2562,7 +2763,7 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="14" t="s">
+      <c r="A46" t="s">
         <v>122</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2573,7 +2774,7 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="14" t="s">
+      <c r="A47" t="s">
         <v>172</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2584,7 +2785,7 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="14" t="s">
+      <c r="A48" t="s">
         <v>124</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2595,7 +2796,7 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="14" t="s">
+      <c r="A49" t="s">
         <v>126</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2606,7 +2807,7 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="14" t="s">
+      <c r="A50" t="s">
         <v>130</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2617,7 +2818,7 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="14" t="s">
+      <c r="A51" t="s">
         <v>173</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2628,7 +2829,7 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="14" t="s">
+      <c r="A52" t="s">
         <v>133</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2639,7 +2840,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="14" t="s">
+      <c r="A53" t="s">
         <v>135</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2650,7 +2851,7 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="14" t="s">
+      <c r="A54" t="s">
         <v>174</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2661,7 +2862,7 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="14" t="s">
+      <c r="A55" t="s">
         <v>175</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2672,7 +2873,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="14" t="s">
+      <c r="A56" t="s">
         <v>176</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2683,7 +2884,7 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="14" t="s">
+      <c r="A57" t="s">
         <v>177</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -2694,7 +2895,7 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="14" t="s">
+      <c r="A58" t="s">
         <v>178</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -2705,7 +2906,7 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="14" t="s">
+      <c r="A59" t="s">
         <v>179</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2716,7 +2917,7 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="14" t="s">
+      <c r="A60" t="s">
         <v>180</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2727,7 +2928,7 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="14" t="s">
+      <c r="A61" t="s">
         <v>181</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -2738,7 +2939,7 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="14" t="s">
+      <c r="A62" t="s">
         <v>182</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -2749,7 +2950,7 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="14" t="s">
+      <c r="A63" t="s">
         <v>183</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -2760,7 +2961,7 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="14" t="s">
+      <c r="A64" t="s">
         <v>184</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -2771,7 +2972,7 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="14" t="s">
+      <c r="A65" t="s">
         <v>185</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2782,7 +2983,7 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="14" t="s">
+      <c r="A66" t="s">
         <v>186</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -2793,7 +2994,7 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="14" t="s">
+      <c r="A67" t="s">
         <v>187</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -2804,7 +3005,7 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="14" t="s">
+      <c r="A68" t="s">
         <v>188</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -2815,7 +3016,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="14" t="s">
+      <c r="A69" t="s">
         <v>189</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2826,7 +3027,7 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="14" t="s">
+      <c r="A70" t="s">
         <v>190</v>
       </c>
       <c r="D70" s="2" t="s">
@@ -2837,7 +3038,7 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="14" t="s">
+      <c r="A71" t="s">
         <v>191</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -2848,7 +3049,7 @@
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="14" t="s">
+      <c r="A72" t="s">
         <v>192</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -2859,7 +3060,7 @@
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="14" t="s">
+      <c r="A73" t="s">
         <v>193</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -2870,7 +3071,7 @@
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="14" t="s">
+      <c r="A74" t="s">
         <v>194</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -2881,7 +3082,7 @@
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="14" t="s">
+      <c r="A75" t="s">
         <v>195</v>
       </c>
       <c r="D75" s="2" t="s">
@@ -2892,7 +3093,7 @@
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="14" t="s">
+      <c r="A76" t="s">
         <v>196</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -2903,7 +3104,7 @@
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="14" t="s">
+      <c r="A77" t="s">
         <v>197</v>
       </c>
       <c r="D77" s="2" t="s">
@@ -2914,7 +3115,7 @@
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="14" t="s">
+      <c r="A78" t="s">
         <v>198</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -2925,7 +3126,7 @@
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="14" t="s">
+      <c r="A79" t="s">
         <v>199</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -2936,7 +3137,7 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="14" t="s">
+      <c r="A80" t="s">
         <v>200</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -2947,7 +3148,7 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="14" t="s">
+      <c r="A81" t="s">
         <v>201</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -2958,7 +3159,7 @@
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="14" t="s">
+      <c r="A82" t="s">
         <v>202</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -2969,7 +3170,7 @@
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="14" t="s">
+      <c r="A83" t="s">
         <v>203</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -2980,7 +3181,7 @@
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="14" t="s">
+      <c r="A84" t="s">
         <v>204</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -2991,7 +3192,7 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="14" t="s">
+      <c r="A85" t="s">
         <v>205</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3002,7 +3203,7 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="14" t="s">
+      <c r="A86" t="s">
         <v>206</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -3013,7 +3214,7 @@
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="14" t="s">
+      <c r="A87" t="s">
         <v>207</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3024,7 +3225,7 @@
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="14" t="s">
+      <c r="A88" t="s">
         <v>208</v>
       </c>
       <c r="D88" s="2" t="s">
@@ -3035,7 +3236,7 @@
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="14" t="s">
+      <c r="A89" t="s">
         <v>209</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3046,7 +3247,7 @@
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="14" t="s">
+      <c r="A90" t="s">
         <v>210</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -3057,7 +3258,7 @@
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="14" t="s">
+      <c r="A91" t="s">
         <v>211</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3068,7 +3269,7 @@
       </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="14" t="s">
+      <c r="A92" t="s">
         <v>212</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -3079,7 +3280,7 @@
       </c>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="14" t="s">
+      <c r="A93" t="s">
         <v>213</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3090,7 +3291,7 @@
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="14" t="s">
+      <c r="A94" t="s">
         <v>214</v>
       </c>
       <c r="D94" s="2" t="s">
@@ -3101,7 +3302,7 @@
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="14" t="s">
+      <c r="A95" t="s">
         <v>215</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3112,7 +3313,7 @@
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="14" t="s">
+      <c r="A96" t="s">
         <v>216</v>
       </c>
       <c r="D96" s="2" t="s">
@@ -3123,7 +3324,7 @@
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="14" t="s">
+      <c r="A97" t="s">
         <v>217</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3134,7 +3335,7 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="14" t="s">
+      <c r="A98" t="s">
         <v>218</v>
       </c>
       <c r="D98" s="2" t="s">
@@ -3145,7 +3346,7 @@
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="14" t="s">
+      <c r="A99" t="s">
         <v>219</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3156,7 +3357,7 @@
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="14" t="s">
+      <c r="A100" t="s">
         <v>220</v>
       </c>
       <c r="D100" s="2" t="s">
@@ -3167,7 +3368,7 @@
       </c>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="14" t="s">
+      <c r="A101" t="s">
         <v>221</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -3178,7 +3379,7 @@
       </c>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="14" t="s">
+      <c r="A102" t="s">
         <v>222</v>
       </c>
       <c r="D102" s="2" t="s">
@@ -3189,7 +3390,7 @@
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="14" t="s">
+      <c r="A103" t="s">
         <v>223</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -3200,7 +3401,7 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="14" t="s">
+      <c r="A104" t="s">
         <v>224</v>
       </c>
       <c r="D104" s="2" t="s">
@@ -3211,7 +3412,7 @@
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="14" t="s">
+      <c r="A105" t="s">
         <v>225</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -3222,7 +3423,7 @@
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="14" t="s">
+      <c r="A106" t="s">
         <v>226</v>
       </c>
       <c r="D106" s="2" t="s">
@@ -3233,7 +3434,7 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="14" t="s">
+      <c r="A107" t="s">
         <v>227</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -3244,7 +3445,7 @@
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="14" t="s">
+      <c r="A108" t="s">
         <v>228</v>
       </c>
       <c r="D108" s="2" t="s">
@@ -3255,7 +3456,7 @@
       </c>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="14" t="s">
+      <c r="A109" t="s">
         <v>229</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -3266,7 +3467,7 @@
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="14" t="s">
+      <c r="A110" t="s">
         <v>230</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -3277,7 +3478,7 @@
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="14" t="s">
+      <c r="A111" t="s">
         <v>231</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -3288,7 +3489,7 @@
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="14" t="s">
+      <c r="A112" t="s">
         <v>232</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -3299,7 +3500,7 @@
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="14" t="s">
+      <c r="A113" t="s">
         <v>233</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -3310,7 +3511,7 @@
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="14" t="s">
+      <c r="A114" t="s">
         <v>234</v>
       </c>
       <c r="D114" s="2" t="s">
@@ -3321,7 +3522,7 @@
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="14" t="s">
+      <c r="A115" t="s">
         <v>235</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -3332,7 +3533,7 @@
       </c>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="14" t="s">
+      <c r="A116" t="s">
         <v>236</v>
       </c>
       <c r="D116" s="2" t="s">
@@ -3343,7 +3544,7 @@
       </c>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="14" t="s">
+      <c r="A117" t="s">
         <v>237</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -3354,7 +3555,7 @@
       </c>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="14" t="s">
+      <c r="A118" t="s">
         <v>238</v>
       </c>
       <c r="D118" s="2" t="s">
@@ -3365,7 +3566,7 @@
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="14" t="s">
+      <c r="A119" t="s">
         <v>239</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -3376,7 +3577,7 @@
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="14" t="s">
+      <c r="A120" t="s">
         <v>240</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -3387,7 +3588,7 @@
       </c>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="14" t="s">
+      <c r="A121" t="s">
         <v>241</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -3398,7 +3599,7 @@
       </c>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="14" t="s">
+      <c r="A122" t="s">
         <v>242</v>
       </c>
       <c r="D122" s="2" t="s">
@@ -3409,7 +3610,7 @@
       </c>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="14" t="s">
+      <c r="A123" t="s">
         <v>243</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -3420,7 +3621,7 @@
       </c>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="14" t="s">
+      <c r="A124" t="s">
         <v>244</v>
       </c>
       <c r="D124" s="2" t="s">
@@ -3431,7 +3632,7 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="14" t="s">
+      <c r="A125" t="s">
         <v>245</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -3442,7 +3643,7 @@
       </c>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="14" t="s">
+      <c r="A126" t="s">
         <v>246</v>
       </c>
       <c r="D126" s="2" t="s">
@@ -3453,7 +3654,7 @@
       </c>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="14" t="s">
+      <c r="A127" t="s">
         <v>247</v>
       </c>
       <c r="D127" s="2" t="s">
@@ -3464,7 +3665,7 @@
       </c>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="14" t="s">
+      <c r="A128" t="s">
         <v>248</v>
       </c>
       <c r="D128" s="2" t="s">
@@ -3475,7 +3676,7 @@
       </c>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="14" t="s">
+      <c r="A129" t="s">
         <v>249</v>
       </c>
       <c r="D129" s="2" t="s">
@@ -3486,7 +3687,7 @@
       </c>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="14" t="s">
+      <c r="A130" t="s">
         <v>250</v>
       </c>
       <c r="D130" s="2" t="s">
@@ -3497,7 +3698,7 @@
       </c>
     </row>
     <row r="131" spans="1:5">
-      <c r="A131" s="14" t="s">
+      <c r="A131" t="s">
         <v>251</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -3508,7 +3709,7 @@
       </c>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="14" t="s">
+      <c r="A132" t="s">
         <v>252</v>
       </c>
       <c r="D132" s="2" t="s">
@@ -3519,7 +3720,7 @@
       </c>
     </row>
     <row r="133" spans="1:5">
-      <c r="A133" s="14" t="s">
+      <c r="A133" t="s">
         <v>253</v>
       </c>
       <c r="D133" s="2" t="s">
@@ -3530,7 +3731,7 @@
       </c>
     </row>
     <row r="134" spans="1:5">
-      <c r="A134" s="14" t="s">
+      <c r="A134" t="s">
         <v>254</v>
       </c>
       <c r="D134" s="2" t="s">
@@ -3541,7 +3742,7 @@
       </c>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="14" t="s">
+      <c r="A135" t="s">
         <v>255</v>
       </c>
       <c r="D135" s="2" t="s">
@@ -3552,7 +3753,7 @@
       </c>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="14" t="s">
+      <c r="A136" t="s">
         <v>256</v>
       </c>
       <c r="D136" s="2" t="s">
@@ -3563,7 +3764,7 @@
       </c>
     </row>
     <row r="137" spans="1:5">
-      <c r="A137" s="14" t="s">
+      <c r="A137" t="s">
         <v>257</v>
       </c>
       <c r="D137" s="2" t="s">
@@ -3574,7 +3775,7 @@
       </c>
     </row>
     <row r="138" spans="1:5">
-      <c r="A138" s="14" t="s">
+      <c r="A138" t="s">
         <v>258</v>
       </c>
       <c r="D138" s="2" t="s">
@@ -3585,7 +3786,7 @@
       </c>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="14" t="s">
+      <c r="A139" t="s">
         <v>259</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -3596,7 +3797,7 @@
       </c>
     </row>
     <row r="140" spans="1:5">
-      <c r="A140" s="14" t="s">
+      <c r="A140" t="s">
         <v>260</v>
       </c>
       <c r="D140" s="2" t="s">
@@ -3607,7 +3808,7 @@
       </c>
     </row>
     <row r="141" spans="1:5">
-      <c r="A141" s="14" t="s">
+      <c r="A141" t="s">
         <v>261</v>
       </c>
       <c r="D141" s="2" t="s">
@@ -3618,7 +3819,7 @@
       </c>
     </row>
     <row r="142" spans="1:5">
-      <c r="A142" s="14" t="s">
+      <c r="A142" t="s">
         <v>262</v>
       </c>
       <c r="D142" s="2" t="s">
@@ -3629,7 +3830,7 @@
       </c>
     </row>
     <row r="143" spans="1:5">
-      <c r="A143" s="14" t="s">
+      <c r="A143" t="s">
         <v>263</v>
       </c>
       <c r="D143" s="2" t="s">
@@ -3640,7 +3841,7 @@
       </c>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="14" t="s">
+      <c r="A144" t="s">
         <v>264</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -3651,7 +3852,7 @@
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="14" t="s">
+      <c r="A145" t="s">
         <v>265</v>
       </c>
       <c r="D145" s="2" t="s">
@@ -3662,7 +3863,7 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="14" t="s">
+      <c r="A146" t="s">
         <v>266</v>
       </c>
       <c r="D146" s="2" t="s">
@@ -3673,7 +3874,7 @@
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="14" t="s">
+      <c r="A147" t="s">
         <v>267</v>
       </c>
       <c r="D147" s="2" t="s">
@@ -3684,7 +3885,7 @@
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="14" t="s">
+      <c r="A148" t="s">
         <v>268</v>
       </c>
       <c r="D148" s="2" t="s">
@@ -3695,7 +3896,7 @@
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="14" t="s">
+      <c r="A149" t="s">
         <v>269</v>
       </c>
       <c r="D149" s="2" t="s">
@@ -3706,7 +3907,7 @@
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="14" t="s">
+      <c r="A150" t="s">
         <v>270</v>
       </c>
       <c r="D150" s="2" t="s">
@@ -3717,7 +3918,7 @@
       </c>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="14" t="s">
+      <c r="A151" t="s">
         <v>271</v>
       </c>
       <c r="D151" s="2" t="s">
@@ -3728,7 +3929,7 @@
       </c>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="14" t="s">
+      <c r="A152" t="s">
         <v>272</v>
       </c>
       <c r="D152" s="2" t="s">
@@ -3739,7 +3940,7 @@
       </c>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="14" t="s">
+      <c r="A153" t="s">
         <v>273</v>
       </c>
       <c r="D153" s="2" t="s">

</xml_diff>

<commit_message>
used columns in silver layer added
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\lending_club_credit_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E4E984-5DEF-4E34-8791-62174A133BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF475F-3AF1-4547-BF0E-C1EC6505F6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Columns" sheetId="1" r:id="rId1"/>
-    <sheet name="Business_rules" sheetId="2" r:id="rId2"/>
-    <sheet name="Data_quality_issues" sheetId="4" r:id="rId3"/>
+    <sheet name="Columns_description" sheetId="1" r:id="rId1"/>
+    <sheet name="profiling_checks" sheetId="5" r:id="rId2"/>
+    <sheet name="Business_rules" sheetId="2" r:id="rId3"/>
+    <sheet name="Data_quality_issues" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Columns_description!$A$1:$H$152</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="389">
   <si>
     <t>Column Name</t>
   </si>
@@ -1256,6 +1260,33 @@
   </si>
   <si>
     <t>Avg Per State</t>
+  </si>
+  <si>
+    <t>start_dt</t>
+  </si>
+  <si>
+    <t>end_dt</t>
+  </si>
+  <si>
+    <t>is_deliquent</t>
+  </si>
+  <si>
+    <t>is_performing</t>
+  </si>
+  <si>
+    <t>is_non_performing</t>
+  </si>
+  <si>
+    <t>is_default</t>
+  </si>
+  <si>
+    <t>is_chargedoff</t>
+  </si>
+  <si>
+    <t>Silver_layer</t>
+  </si>
+  <si>
+    <t>Used</t>
   </si>
 </sst>
 </file>
@@ -1991,13 +2022,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -2385,10 +2416,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F950F64-58AC-4A83-B722-8F79BA8F22E8}">
-  <dimension ref="A1:F152"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2401,7 +2433,7 @@
     <col min="6" max="6" width="44.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1">
+    <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2420,8 +2452,14 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2440,8 +2478,15 @@
       <c r="F2" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="str">
+        <f>IF(ISNUMBER(MATCH(A2, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -2458,8 +2503,15 @@
       <c r="F3" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="str">
+        <f>IF(ISNUMBER(MATCH(A3, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2478,8 +2530,15 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="str">
+        <f>IF(ISNUMBER(MATCH(A4, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
@@ -2498,8 +2557,15 @@
       <c r="F5" s="9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="str">
+        <f>IF(ISNUMBER(MATCH(A5, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="9" t="s">
         <v>49</v>
       </c>
@@ -2518,8 +2584,15 @@
       <c r="F6" s="9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="str">
+        <f>IF(ISNUMBER(MATCH(A6, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2538,8 +2611,15 @@
       <c r="F7" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="str">
+        <f>IF(ISNUMBER(MATCH(A7, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2558,8 +2638,15 @@
       <c r="F8" s="10" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="str">
+        <f>IF(ISNUMBER(MATCH(A8, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2578,8 +2665,15 @@
       <c r="F9" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="str">
+        <f>IF(ISNUMBER(MATCH(A9, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2598,8 +2692,15 @@
       <c r="F10" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="str">
+        <f>IF(ISNUMBER(MATCH(A10, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2618,8 +2719,15 @@
       <c r="F11" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="str">
+        <f>IF(ISNUMBER(MATCH(A11, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2638,8 +2746,15 @@
       <c r="F12" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="str">
+        <f>IF(ISNUMBER(MATCH(A12, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2658,8 +2773,15 @@
       <c r="F13" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="str">
+        <f>IF(ISNUMBER(MATCH(A13, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2678,8 +2800,15 @@
       <c r="F14" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="str">
+        <f>IF(ISNUMBER(MATCH(A14, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2698,8 +2827,15 @@
       <c r="F15" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="str">
+        <f>IF(ISNUMBER(MATCH(A15, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2718,8 +2854,15 @@
       <c r="F16" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="str">
+        <f>IF(ISNUMBER(MATCH(A16, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2738,8 +2881,15 @@
       <c r="F17" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="str">
+        <f>IF(ISNUMBER(MATCH(A17, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2758,8 +2908,15 @@
       <c r="F18" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="str">
+        <f>IF(ISNUMBER(MATCH(A18, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2778,8 +2935,15 @@
       <c r="F19" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="str">
+        <f>IF(ISNUMBER(MATCH(A19, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2798,8 +2962,15 @@
       <c r="F20" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="str">
+        <f>IF(ISNUMBER(MATCH(A20, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2815,8 +2986,15 @@
       <c r="F21" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="str">
+        <f>IF(ISNUMBER(MATCH(A21, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H21" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2835,8 +3013,15 @@
       <c r="F22" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" t="str">
+        <f>IF(ISNUMBER(MATCH(A22, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -2855,8 +3040,15 @@
       <c r="F23" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="str">
+        <f>IF(ISNUMBER(MATCH(A23, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H23" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -2875,8 +3067,15 @@
       <c r="F24" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="str">
+        <f>IF(ISNUMBER(MATCH(A24, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H24" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2895,8 +3094,15 @@
       <c r="F25" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="28.5">
+      <c r="G25" t="str">
+        <f>IF(ISNUMBER(MATCH(A25, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.5">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2915,8 +3121,15 @@
       <c r="F26" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" t="str">
+        <f>IF(ISNUMBER(MATCH(A26, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H26" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2935,8 +3148,15 @@
       <c r="F27" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" t="str">
+        <f>IF(ISNUMBER(MATCH(A27, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H27" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2955,8 +3175,15 @@
       <c r="F28" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" t="str">
+        <f>IF(ISNUMBER(MATCH(A28, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2975,8 +3202,15 @@
       <c r="F29" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" t="str">
+        <f>IF(ISNUMBER(MATCH(A29, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2995,8 +3229,15 @@
       <c r="F30" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" t="str">
+        <f>IF(ISNUMBER(MATCH(A30, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -3015,8 +3256,15 @@
       <c r="F31" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" t="str">
+        <f>IF(ISNUMBER(MATCH(A31, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -3035,8 +3283,15 @@
       <c r="F32" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" t="str">
+        <f>IF(ISNUMBER(MATCH(A32, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -3055,8 +3310,15 @@
       <c r="F33" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" t="str">
+        <f>IF(ISNUMBER(MATCH(A33, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -3075,8 +3337,15 @@
       <c r="F34" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" t="str">
+        <f>IF(ISNUMBER(MATCH(A34, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -3095,8 +3364,15 @@
       <c r="F35" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" t="str">
+        <f>IF(ISNUMBER(MATCH(A35, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -3115,8 +3391,15 @@
       <c r="F36" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.5">
+      <c r="G36" t="str">
+        <f>IF(ISNUMBER(MATCH(A36, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.5">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -3135,8 +3418,15 @@
       <c r="F37" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" t="str">
+        <f>IF(ISNUMBER(MATCH(A37, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3155,8 +3445,15 @@
       <c r="F38" s="10" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" t="str">
+        <f>IF(ISNUMBER(MATCH(A38, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -3175,8 +3472,15 @@
       <c r="F39" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" t="str">
+        <f>IF(ISNUMBER(MATCH(A39, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -3195,8 +3499,15 @@
       <c r="F40" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40" t="str">
+        <f>IF(ISNUMBER(MATCH(A40, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -3215,8 +3526,15 @@
       <c r="F41" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" t="str">
+        <f>IF(ISNUMBER(MATCH(A41, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3235,8 +3553,15 @@
       <c r="F42" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" t="str">
+        <f>IF(ISNUMBER(MATCH(A42, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -3255,8 +3580,15 @@
       <c r="F43" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" t="str">
+        <f>IF(ISNUMBER(MATCH(A43, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -3275,8 +3607,15 @@
       <c r="F44" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" t="str">
+        <f>IF(ISNUMBER(MATCH(A44, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3295,8 +3634,15 @@
       <c r="F45" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" t="str">
+        <f>IF(ISNUMBER(MATCH(A45, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -3315,8 +3661,15 @@
       <c r="F46" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" t="str">
+        <f>IF(ISNUMBER(MATCH(A46, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -3335,8 +3688,15 @@
       <c r="F47" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" t="str">
+        <f>IF(ISNUMBER(MATCH(A47, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -3355,8 +3715,15 @@
       <c r="F48" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="27.4">
+      <c r="G48" t="str">
+        <f>IF(ISNUMBER(MATCH(A48, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="27.4" hidden="1">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3375,8 +3742,15 @@
       <c r="F49" s="11" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" t="str">
+        <f>IF(ISNUMBER(MATCH(A49, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -3395,8 +3769,15 @@
       <c r="F50" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" t="str">
+        <f>IF(ISNUMBER(MATCH(A50, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" hidden="1">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -3415,8 +3796,15 @@
       <c r="F51" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" t="str">
+        <f>IF(ISNUMBER(MATCH(A51, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" hidden="1">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -3435,8 +3823,15 @@
       <c r="F52" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" t="str">
+        <f>IF(ISNUMBER(MATCH(A52, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -3455,8 +3850,15 @@
       <c r="F53" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" t="str">
+        <f>IF(ISNUMBER(MATCH(A53, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -3475,8 +3877,15 @@
       <c r="F54" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" t="str">
+        <f>IF(ISNUMBER(MATCH(A54, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+      <c r="H54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" hidden="1">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -3495,8 +3904,15 @@
       <c r="F55" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55" t="str">
+        <f>IF(ISNUMBER(MATCH(A55, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" hidden="1">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -3515,8 +3931,15 @@
       <c r="F56" s="5" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56" t="str">
+        <f>IF(ISNUMBER(MATCH(A56, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -3535,8 +3958,12 @@
       <c r="F57" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" t="str">
+        <f>IF(ISNUMBER(MATCH(A57, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -3555,8 +3982,12 @@
       <c r="F58" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" t="str">
+        <f>IF(ISNUMBER(MATCH(A58, H:H, 0)), "Y", "N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" hidden="1">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -3575,8 +4006,12 @@
       <c r="F59" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" t="str">
+        <f>IF(ISNUMBER(MATCH(A59, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -3595,8 +4030,12 @@
       <c r="F60" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" t="str">
+        <f>IF(ISNUMBER(MATCH(A60, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -3615,8 +4054,12 @@
       <c r="F61" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" t="str">
+        <f>IF(ISNUMBER(MATCH(A61, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3635,8 +4078,12 @@
       <c r="F62" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" t="str">
+        <f>IF(ISNUMBER(MATCH(A62, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -3655,8 +4102,12 @@
       <c r="F63" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" t="str">
+        <f>IF(ISNUMBER(MATCH(A63, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -3675,8 +4126,12 @@
       <c r="F64" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64" t="str">
+        <f>IF(ISNUMBER(MATCH(A64, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3695,8 +4150,12 @@
       <c r="F65" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" t="str">
+        <f>IF(ISNUMBER(MATCH(A65, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -3715,8 +4174,12 @@
       <c r="F66" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66" t="str">
+        <f>IF(ISNUMBER(MATCH(A66, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -3735,8 +4198,12 @@
       <c r="F67" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67" t="str">
+        <f>IF(ISNUMBER(MATCH(A67, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -3755,8 +4222,12 @@
       <c r="F68" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68" t="str">
+        <f>IF(ISNUMBER(MATCH(A68, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -3775,8 +4246,12 @@
       <c r="F69" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69" t="str">
+        <f>IF(ISNUMBER(MATCH(A69, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -3795,8 +4270,12 @@
       <c r="F70" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70" t="str">
+        <f>IF(ISNUMBER(MATCH(A70, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -3815,8 +4294,12 @@
       <c r="F71" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71" t="str">
+        <f>IF(ISNUMBER(MATCH(A71, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" t="s">
         <v>89</v>
       </c>
@@ -3835,8 +4318,12 @@
       <c r="F72" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" t="str">
+        <f>IF(ISNUMBER(MATCH(A72, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" t="s">
         <v>90</v>
       </c>
@@ -3855,8 +4342,12 @@
       <c r="F73" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73" t="str">
+        <f>IF(ISNUMBER(MATCH(A73, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -3875,8 +4366,12 @@
       <c r="F74" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74" t="str">
+        <f>IF(ISNUMBER(MATCH(A74, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1">
       <c r="A75" t="s">
         <v>92</v>
       </c>
@@ -3895,8 +4390,12 @@
       <c r="F75" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75" t="str">
+        <f>IF(ISNUMBER(MATCH(A75, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -3915,8 +4414,12 @@
       <c r="F76" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76" t="str">
+        <f>IF(ISNUMBER(MATCH(A76, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -3935,8 +4438,12 @@
       <c r="F77" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77" t="str">
+        <f>IF(ISNUMBER(MATCH(A77, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1">
       <c r="A78" t="s">
         <v>95</v>
       </c>
@@ -3955,8 +4462,12 @@
       <c r="F78" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78" t="str">
+        <f>IF(ISNUMBER(MATCH(A78, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -3975,8 +4486,12 @@
       <c r="F79" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79" t="str">
+        <f>IF(ISNUMBER(MATCH(A79, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1">
       <c r="A80" t="s">
         <v>97</v>
       </c>
@@ -3995,8 +4510,12 @@
       <c r="F80" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80" t="str">
+        <f>IF(ISNUMBER(MATCH(A80, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" t="s">
         <v>98</v>
       </c>
@@ -4015,8 +4534,12 @@
       <c r="F81" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81" t="str">
+        <f>IF(ISNUMBER(MATCH(A81, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" t="s">
         <v>99</v>
       </c>
@@ -4035,8 +4558,12 @@
       <c r="F82" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82" t="str">
+        <f>IF(ISNUMBER(MATCH(A82, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -4055,8 +4582,12 @@
       <c r="F83" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83" t="str">
+        <f>IF(ISNUMBER(MATCH(A83, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -4075,8 +4606,12 @@
       <c r="F84" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84" t="str">
+        <f>IF(ISNUMBER(MATCH(A84, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -4095,8 +4630,12 @@
       <c r="F85" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85" t="str">
+        <f>IF(ISNUMBER(MATCH(A85, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -4115,8 +4654,12 @@
       <c r="F86" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86" t="str">
+        <f>IF(ISNUMBER(MATCH(A86, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -4135,8 +4678,12 @@
       <c r="F87" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87" t="str">
+        <f>IF(ISNUMBER(MATCH(A87, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1">
       <c r="A88" t="s">
         <v>105</v>
       </c>
@@ -4155,8 +4702,12 @@
       <c r="F88" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88" t="str">
+        <f>IF(ISNUMBER(MATCH(A88, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" t="s">
         <v>106</v>
       </c>
@@ -4175,8 +4726,12 @@
       <c r="F89" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89" t="str">
+        <f>IF(ISNUMBER(MATCH(A89, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -4195,8 +4750,12 @@
       <c r="F90" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90" t="str">
+        <f>IF(ISNUMBER(MATCH(A90, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" t="s">
         <v>108</v>
       </c>
@@ -4215,8 +4774,12 @@
       <c r="F91" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91" t="str">
+        <f>IF(ISNUMBER(MATCH(A91, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" hidden="1">
       <c r="A92" t="s">
         <v>109</v>
       </c>
@@ -4235,8 +4798,12 @@
       <c r="F92" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92" t="str">
+        <f>IF(ISNUMBER(MATCH(A92, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1">
       <c r="A93" t="s">
         <v>110</v>
       </c>
@@ -4255,8 +4822,12 @@
       <c r="F93" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93" t="str">
+        <f>IF(ISNUMBER(MATCH(A93, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" t="s">
         <v>111</v>
       </c>
@@ -4275,8 +4846,12 @@
       <c r="F94" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94" t="str">
+        <f>IF(ISNUMBER(MATCH(A94, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -4295,8 +4870,12 @@
       <c r="F95" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95" t="str">
+        <f>IF(ISNUMBER(MATCH(A95, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" hidden="1">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -4315,8 +4894,12 @@
       <c r="F96" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96" t="str">
+        <f>IF(ISNUMBER(MATCH(A96, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -4335,8 +4918,12 @@
       <c r="F97" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97" t="str">
+        <f>IF(ISNUMBER(MATCH(A97, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -4355,8 +4942,12 @@
       <c r="F98" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98" t="str">
+        <f>IF(ISNUMBER(MATCH(A98, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -4375,8 +4966,12 @@
       <c r="F99" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99" t="str">
+        <f>IF(ISNUMBER(MATCH(A99, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -4395,8 +4990,12 @@
       <c r="F100" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100" t="str">
+        <f>IF(ISNUMBER(MATCH(A100, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1">
       <c r="A101" t="s">
         <v>118</v>
       </c>
@@ -4415,8 +5014,12 @@
       <c r="F101" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101" t="str">
+        <f>IF(ISNUMBER(MATCH(A101, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" hidden="1">
       <c r="A102" t="s">
         <v>119</v>
       </c>
@@ -4435,8 +5038,12 @@
       <c r="F102" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102" t="str">
+        <f>IF(ISNUMBER(MATCH(A102, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" t="s">
         <v>120</v>
       </c>
@@ -4455,8 +5062,12 @@
       <c r="F103" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103" t="str">
+        <f>IF(ISNUMBER(MATCH(A103, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" hidden="1">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -4475,8 +5086,12 @@
       <c r="F104" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104" t="str">
+        <f>IF(ISNUMBER(MATCH(A104, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" hidden="1">
       <c r="A105" t="s">
         <v>122</v>
       </c>
@@ -4495,8 +5110,12 @@
       <c r="F105" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105" t="str">
+        <f>IF(ISNUMBER(MATCH(A105, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" t="s">
         <v>123</v>
       </c>
@@ -4515,8 +5134,12 @@
       <c r="F106" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106" t="str">
+        <f>IF(ISNUMBER(MATCH(A106, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1">
       <c r="A107" t="s">
         <v>124</v>
       </c>
@@ -4535,8 +5158,12 @@
       <c r="F107" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107" t="str">
+        <f>IF(ISNUMBER(MATCH(A107, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" t="s">
         <v>125</v>
       </c>
@@ -4555,8 +5182,12 @@
       <c r="F108" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108" t="str">
+        <f>IF(ISNUMBER(MATCH(A108, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" t="s">
         <v>126</v>
       </c>
@@ -4575,8 +5206,12 @@
       <c r="F109" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109" t="str">
+        <f>IF(ISNUMBER(MATCH(A109, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" hidden="1">
       <c r="A110" t="s">
         <v>127</v>
       </c>
@@ -4595,8 +5230,12 @@
       <c r="F110" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110" t="str">
+        <f>IF(ISNUMBER(MATCH(A110, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" hidden="1">
       <c r="A111" t="s">
         <v>128</v>
       </c>
@@ -4615,8 +5254,12 @@
       <c r="F111" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111" t="str">
+        <f>IF(ISNUMBER(MATCH(A111, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -4635,8 +5278,12 @@
       <c r="F112" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112" t="str">
+        <f>IF(ISNUMBER(MATCH(A112, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" t="s">
         <v>130</v>
       </c>
@@ -4655,8 +5302,12 @@
       <c r="F113" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113" t="str">
+        <f>IF(ISNUMBER(MATCH(A113, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" t="s">
         <v>131</v>
       </c>
@@ -4675,8 +5326,12 @@
       <c r="F114" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114" t="str">
+        <f>IF(ISNUMBER(MATCH(A114, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" t="s">
         <v>132</v>
       </c>
@@ -4695,8 +5350,12 @@
       <c r="F115" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115" t="str">
+        <f>IF(ISNUMBER(MATCH(A115, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" hidden="1">
       <c r="A116" t="s">
         <v>133</v>
       </c>
@@ -4715,8 +5374,12 @@
       <c r="F116" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116" t="str">
+        <f>IF(ISNUMBER(MATCH(A116, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" t="s">
         <v>134</v>
       </c>
@@ -4735,8 +5398,12 @@
       <c r="F117" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117" t="str">
+        <f>IF(ISNUMBER(MATCH(A117, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -4755,8 +5422,12 @@
       <c r="F118" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118" t="str">
+        <f>IF(ISNUMBER(MATCH(A118, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" t="s">
         <v>136</v>
       </c>
@@ -4775,8 +5446,12 @@
       <c r="F119" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119" t="str">
+        <f>IF(ISNUMBER(MATCH(A119, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" t="s">
         <v>137</v>
       </c>
@@ -4795,8 +5470,12 @@
       <c r="F120" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120" t="str">
+        <f>IF(ISNUMBER(MATCH(A120, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" hidden="1">
       <c r="A121" t="s">
         <v>138</v>
       </c>
@@ -4815,8 +5494,12 @@
       <c r="F121" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121" t="str">
+        <f>IF(ISNUMBER(MATCH(A121, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" t="s">
         <v>139</v>
       </c>
@@ -4835,8 +5518,12 @@
       <c r="F122" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122" t="str">
+        <f>IF(ISNUMBER(MATCH(A122, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" t="s">
         <v>140</v>
       </c>
@@ -4855,8 +5542,12 @@
       <c r="F123" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123" t="str">
+        <f>IF(ISNUMBER(MATCH(A123, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -4875,8 +5566,12 @@
       <c r="F124" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124" t="str">
+        <f>IF(ISNUMBER(MATCH(A124, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -4895,8 +5590,12 @@
       <c r="F125" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125" t="str">
+        <f>IF(ISNUMBER(MATCH(A125, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" t="s">
         <v>143</v>
       </c>
@@ -4915,8 +5614,12 @@
       <c r="F126" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126" t="str">
+        <f>IF(ISNUMBER(MATCH(A126, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" t="s">
         <v>144</v>
       </c>
@@ -4935,8 +5638,12 @@
       <c r="F127" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127" t="str">
+        <f>IF(ISNUMBER(MATCH(A127, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" t="s">
         <v>145</v>
       </c>
@@ -4955,8 +5662,12 @@
       <c r="F128" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128" t="str">
+        <f>IF(ISNUMBER(MATCH(A128, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -4975,8 +5686,12 @@
       <c r="F129" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129" t="str">
+        <f>IF(ISNUMBER(MATCH(A129, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" t="s">
         <v>147</v>
       </c>
@@ -4995,8 +5710,12 @@
       <c r="F130" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130" t="str">
+        <f>IF(ISNUMBER(MATCH(A130, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" t="s">
         <v>148</v>
       </c>
@@ -5015,8 +5734,12 @@
       <c r="F131" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131" t="str">
+        <f>IF(ISNUMBER(MATCH(A131, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -5035,8 +5758,12 @@
       <c r="F132" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132" t="str">
+        <f>IF(ISNUMBER(MATCH(A132, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" t="s">
         <v>150</v>
       </c>
@@ -5055,8 +5782,12 @@
       <c r="F133" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133" t="str">
+        <f>IF(ISNUMBER(MATCH(A133, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" t="s">
         <v>151</v>
       </c>
@@ -5075,8 +5806,12 @@
       <c r="F134" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134" t="str">
+        <f>IF(ISNUMBER(MATCH(A134, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" t="s">
         <v>152</v>
       </c>
@@ -5095,8 +5830,12 @@
       <c r="F135" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135" t="str">
+        <f>IF(ISNUMBER(MATCH(A135, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" hidden="1">
       <c r="A136" t="s">
         <v>153</v>
       </c>
@@ -5115,8 +5854,12 @@
       <c r="F136" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="G136" t="str">
+        <f>IF(ISNUMBER(MATCH(A136, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" t="s">
         <v>154</v>
       </c>
@@ -5135,8 +5878,12 @@
       <c r="F137" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="G137" t="str">
+        <f>IF(ISNUMBER(MATCH(A137, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" t="s">
         <v>155</v>
       </c>
@@ -5155,8 +5902,12 @@
       <c r="F138" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138" t="str">
+        <f>IF(ISNUMBER(MATCH(A138, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1">
       <c r="A139" t="s">
         <v>156</v>
       </c>
@@ -5175,8 +5926,12 @@
       <c r="F139" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="G139" t="str">
+        <f>IF(ISNUMBER(MATCH(A139, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" hidden="1">
       <c r="A140" t="s">
         <v>157</v>
       </c>
@@ -5195,8 +5950,12 @@
       <c r="F140" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="G140" t="str">
+        <f>IF(ISNUMBER(MATCH(A140, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" t="s">
         <v>158</v>
       </c>
@@ -5215,8 +5974,12 @@
       <c r="F141" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="G141" t="str">
+        <f>IF(ISNUMBER(MATCH(A141, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" t="s">
         <v>159</v>
       </c>
@@ -5235,8 +5998,12 @@
       <c r="F142" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="G142" t="str">
+        <f>IF(ISNUMBER(MATCH(A142, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1">
       <c r="A143" t="s">
         <v>160</v>
       </c>
@@ -5255,8 +6022,12 @@
       <c r="F143" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="G143" t="str">
+        <f>IF(ISNUMBER(MATCH(A143, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -5275,8 +6046,12 @@
       <c r="F144" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144" t="str">
+        <f>IF(ISNUMBER(MATCH(A144, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" hidden="1">
       <c r="A145" t="s">
         <v>162</v>
       </c>
@@ -5295,8 +6070,12 @@
       <c r="F145" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="G145" t="str">
+        <f>IF(ISNUMBER(MATCH(A145, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -5315,8 +6094,12 @@
       <c r="F146" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="G146" t="str">
+        <f>IF(ISNUMBER(MATCH(A146, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" hidden="1">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -5335,8 +6118,12 @@
       <c r="F147" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="G147" t="str">
+        <f>IF(ISNUMBER(MATCH(A147, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" hidden="1">
       <c r="A148" t="s">
         <v>165</v>
       </c>
@@ -5355,8 +6142,12 @@
       <c r="F148" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="G148" t="str">
+        <f>IF(ISNUMBER(MATCH(A148, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" hidden="1">
       <c r="A149" t="s">
         <v>166</v>
       </c>
@@ -5375,8 +6166,12 @@
       <c r="F149" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149" t="str">
+        <f>IF(ISNUMBER(MATCH(A149, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" hidden="1">
       <c r="A150" t="s">
         <v>167</v>
       </c>
@@ -5395,8 +6190,12 @@
       <c r="F150" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="G150" t="str">
+        <f>IF(ISNUMBER(MATCH(A150, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" hidden="1">
       <c r="A151" t="s">
         <v>168</v>
       </c>
@@ -5415,8 +6214,12 @@
       <c r="F151" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="G151" t="str">
+        <f>IF(ISNUMBER(MATCH(A151, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" hidden="1">
       <c r="A152" t="s">
         <v>169</v>
       </c>
@@ -5435,18 +6238,287 @@
       <c r="F152" t="s">
         <v>53</v>
       </c>
+      <c r="G152" t="str">
+        <f>IF(ISNUMBER(MATCH(A152, H:H, 0)), "Y", "N")</f>
+        <v>N</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H152" xr:uid="{3F950F64-58AC-4A83-B722-8F79BA8F22E8}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5775640E-8023-4E82-86E7-18CF3F672339}">
+  <dimension ref="A1:A48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="19.3984375" style="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D11E4F-5CC3-4428-AB5D-389AF84DFF0B}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -5651,7 +6723,7 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="29" t="s">
         <v>371</v>
       </c>
       <c r="B17" s="28" t="s">
@@ -5659,7 +6731,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.5">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="30" t="s">
         <v>374</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -5670,7 +6742,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="31" t="s">
         <v>375</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -5684,7 +6756,7 @@
       <c r="A20" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" t="s">
         <v>378</v>
       </c>
       <c r="C20" s="1"/>
@@ -5791,47 +6863,35 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5841,7 +6901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2584BD-CB73-4635-8B03-11F5D5C3DF7C}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>

<commit_message>
profiling the file in brinze layer
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\lending_club_credit_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF475F-3AF1-4547-BF0E-C1EC6505F6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26785EE3-1B24-4A0D-A124-497E81726C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns_description" sheetId="1" r:id="rId1"/>
     <sheet name="profiling_checks" sheetId="5" r:id="rId2"/>
     <sheet name="Business_rules" sheetId="2" r:id="rId3"/>
     <sheet name="Data_quality_issues" sheetId="4" r:id="rId4"/>
+    <sheet name="tmp" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Columns_description!$A$1:$H$152</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="443">
   <si>
     <t>Column Name</t>
   </si>
@@ -1283,10 +1284,172 @@
     <t>is_chargedoff</t>
   </si>
   <si>
-    <t>Silver_layer</t>
-  </si>
-  <si>
     <t>Used</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Null_precentage</t>
+  </si>
+  <si>
+    <t>Distinct_count</t>
+  </si>
+  <si>
+    <t>Silver_layer_lookup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("id", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("member_id", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("funded_amnt", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("funded_amnt_inv", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("term", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("int_rate", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("installment", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("grade", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("sub_grade", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("emp_title", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("emp_length", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("home_ownership", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("annual_inc", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("verification_status", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("issue_d", DateType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("loan_status", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("purpose", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("title", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("zip_code", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("addr_state", StringType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("dti", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("delinq_2yrs", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("earliest_cr_line", DateType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("fico_range_low", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("fico_range_high", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("inq_last_6mths", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("mths_since_last_delinq", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("mths_since_last_record", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("open_acc", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("pub_rec", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("revol_bal", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("revol_util", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_acc", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("initial_list_status", StringType(), True),  # CharType not available, use StringType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("out_prncp", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("out_prncp_inv", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_pymnt", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_pymnt_inv", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_rec_prncp", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_rec_int", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("total_rec_late_fee", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("recoveries", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("collection_recovery_fee", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("last_pymnt_amnt", DecimalType(10,2), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("last_fico_range_high", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("last_fico_range_low", IntegerType(), True),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("policy_code", StringType(), True),  # CharType not available, use StringType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    StructField("application_type", StringType(), True)</t>
+  </si>
+  <si>
+    <t>id,member_id,loan_amnt,funded_amnt,funded_amnt_inv,term,int_rate,installment,grade,sub_grade,emp_title,emp_length,home_ownership,annual_inc,verification_status,issue_d,loan_status,pymnt_plan,url,desc,purpose,title,zip_code,addr_state,dti,delinq_2yrs,earliest_cr_line,fico_range_low,fico_range_high,inq_last_6mths,mths_since_last_delinq,mths_since_last_record,open_acc,pub_rec,revol_bal,revol_util,total_acc,initial_list_status,out_prncp,out_prncp_inv,total_pymnt,total_pymnt_inv,total_rec_prncp,total_rec_int,total_rec_late_fee,recoveries,collection_recovery_fee,last_pymnt_d,last_pymnt_amnt,next_pymnt_d,last_credit_pull_d,last_fico_range_high,last_fico_range_low,collections_12_mths_ex_med,mths_since_last_major_derog,policy_code,application_type,annual_inc_joint,dti_joint,verification_status_joint,acc_now_delinq,tot_coll_amt,tot_cur_bal,open_acc_6m,open_act_il,open_il_12m,open_il_24m,mths_since_rcnt_il,total_bal_il,il_util,open_rv_12m,open_rv_24m,max_bal_bc,all_util,total_rev_hi_lim,inq_fi,total_cu_tl,inq_last_12m,acc_open_past_24mths,avg_cur_bal,bc_open_to_buy,bc_util,chargeoff_within_12_mths,delinq_amnt,mo_sin_old_il_acct,mo_sin_old_rev_tl_op,mo_sin_rcnt_rev_tl_op,mo_sin_rcnt_tl,mort_acc,mths_since_recent_bc,mths_since_recent_bc_dlq,mths_since_recent_inq,mths_since_recent_revol_delinq,num_accts_ever_120_pd,num_actv_bc_tl,num_actv_rev_tl,num_bc_sats,num_bc_tl,num_il_tl,num_op_rev_tl,num_rev_accts,num_rev_tl_bal_gt_0,num_sats,num_tl_120dpd_2m,num_tl_30dpd,num_tl_90g_dpd_24m,num_tl_op_past_12m,pct_tl_nvr_dlq,percent_bc_gt_75,pub_rec_bankruptcies,tax_liens,tot_hi_cred_lim,total_bal_ex_mort,total_bc_limit,total_il_high_credit_limit,revol_bal_joint,sec_app_fico_range_low,sec_app_fico_range_high,sec_app_earliest_cr_line,sec_app_inq_last_6mths,sec_app_mort_acc,sec_app_open_acc,sec_app_revol_util,sec_app_open_act_il,sec_app_num_rev_accts,sec_app_chargeoff_within_12_mths,sec_app_collections_12_mths_ex_med,sec_app_mths_since_last_major_derog,hardship_flag,hardship_type,hardship_reason,hardship_status,deferral_term,hardship_amount,hardship_start_date,hardship_end_date,payment_plan_start_date,hardship_length,hardship_dpd,hardship_loan_status,orig_projected_additional_accrued_interest,hardship_payoff_balance_amount,hardship_last_payment_amount,disbursement_method,debt_settlement_flag,debt_settlement_flag_date,settlement_status,settlement_date,settlement_amount,settlement_percentage,settlement_term</t>
+  </si>
+  <si>
+    <t>68407277,,3600.0,3600.0,3600.0, 36 months,13.99,123.03,C,C4,leadman,10+ years,MORTGAGE,55000.0,Not Verified,Dec-2015,Fully Paid,n,https://lendingclub.com/browse/loanDetail.action?loan_id=68407277,,debt_consolidation,Debt consolidation,190xx,PA,5.91,0.0,Aug-2003,675.0,679.0,1.0,30.0,,7.0,0.0,2765.0,29.7,13.0,w,0.0,0.0,4421.723916800001,4421.72,3600.0,821.72,0.0,0.0,0.0,Jan-2019,122.67,,Mar-2019,564.0,560.0,0.0,30.0,1.0,Individual,,,,0.0,722.0,144904.0,2.0,2.0,0.0,1.0,21.0,4981.0,36.0,3.0,3.0,722.0,34.0,9300.0,3.0,1.0,4.0,4.0,20701.0,1506.0,37.2,0.0,0.0,148.0,128.0,3.0,3.0,1.0,4.0,69.0,4.0,69.0,2.0,2.0,4.0,2.0,5.0,3.0,4.0,9.0,4.0,7.0,0.0,0.0,0.0,3.0,76.9,0.0,0.0,0.0,178050.0,7746.0,2400.0,13734.0,,,,,,,,,,,,,,N,,,,,,,,,,,,,,,Cash,N,,,,,,</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1897,6 +2060,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1943,7 +2119,7 @@
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1956,9 +2132,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2029,6 +2202,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -2419,22 +2599,23 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.59765625" customWidth="1"/>
+    <col min="1" max="1" width="33.59765625" style="33" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="18.19921875" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.86328125" customWidth="1"/>
     <col min="6" max="6" width="44.9296875" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -2452,15 +2633,15 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
-        <v>388</v>
-      </c>
-      <c r="H1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>387</v>
       </c>
+      <c r="H1" s="31" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2487,7 +2668,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1"/>
@@ -2539,10 +2720,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="35" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2554,7 +2735,7 @@
       <c r="E5" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="G5" t="str">
@@ -2566,10 +2747,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="35" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2581,7 +2762,7 @@
       <c r="E6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>201</v>
       </c>
       <c r="G6" t="str">
@@ -2593,7 +2774,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="A7" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -2620,7 +2801,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="A8" s="33" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -2635,7 +2816,7 @@
       <c r="E8" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G8" t="str">
@@ -2647,7 +2828,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
+      <c r="A9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2674,7 +2855,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="A10" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2701,7 +2882,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s">
+      <c r="A11" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2728,7 +2909,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="A12" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2755,7 +2936,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="A13" s="33" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2782,7 +2963,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="A14" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2809,7 +2990,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="A15" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2836,7 +3017,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="A16" s="33" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
@@ -2863,7 +3044,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="A17" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2890,7 +3071,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="s">
+      <c r="A18" s="33" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2995,7 +3176,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="A22" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
@@ -3022,7 +3203,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" t="s">
+      <c r="A23" s="33" t="s">
         <v>58</v>
       </c>
       <c r="B23" t="s">
@@ -3049,7 +3230,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="A24" s="33" t="s">
         <v>59</v>
       </c>
       <c r="B24" t="s">
@@ -3076,7 +3257,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="A25" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
@@ -3103,10 +3284,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.5">
-      <c r="A26" t="s">
+      <c r="A26" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="35" t="s">
         <v>341</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -3130,7 +3311,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" t="s">
+      <c r="A27" s="33" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
@@ -3157,7 +3338,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" t="s">
+      <c r="A28" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B28" t="s">
@@ -3184,7 +3365,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" t="s">
+      <c r="A29" s="33" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
@@ -3211,7 +3392,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" t="s">
+      <c r="A30" s="33" t="s">
         <v>33</v>
       </c>
       <c r="B30" t="s">
@@ -3238,7 +3419,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" t="s">
+      <c r="A31" s="33" t="s">
         <v>61</v>
       </c>
       <c r="B31" t="s">
@@ -3265,7 +3446,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" t="s">
+      <c r="A32" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B32" t="s">
@@ -3292,10 +3473,10 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
+      <c r="A33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="35" t="s">
         <v>214</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -3319,7 +3500,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
+      <c r="A34" s="33" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
@@ -3346,7 +3527,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" t="s">
+      <c r="A35" s="33" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
@@ -3373,7 +3554,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" t="s">
+      <c r="A36" s="33" t="s">
         <v>64</v>
       </c>
       <c r="B36" t="s">
@@ -3400,7 +3581,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="28.5">
-      <c r="A37" t="s">
+      <c r="A37" s="33" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
@@ -3427,7 +3608,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" t="s">
+      <c r="A38" s="33" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -3442,7 +3623,7 @@
       <c r="E38" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>219</v>
       </c>
       <c r="G38" t="str">
@@ -3454,7 +3635,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" t="s">
+      <c r="A39" s="33" t="s">
         <v>65</v>
       </c>
       <c r="B39" t="s">
@@ -3481,7 +3662,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" t="s">
+      <c r="A40" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
@@ -3508,7 +3689,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" t="s">
+      <c r="A41" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B41" t="s">
@@ -3535,7 +3716,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" t="s">
+      <c r="A42" s="33" t="s">
         <v>39</v>
       </c>
       <c r="B42" t="s">
@@ -3562,7 +3743,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" t="s">
+      <c r="A43" s="33" t="s">
         <v>67</v>
       </c>
       <c r="B43" t="s">
@@ -3589,7 +3770,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" t="s">
+      <c r="A44" s="33" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
@@ -3616,7 +3797,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" t="s">
+      <c r="A45" s="33" t="s">
         <v>41</v>
       </c>
       <c r="B45" t="s">
@@ -3643,7 +3824,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" t="s">
+      <c r="A46" s="33" t="s">
         <v>68</v>
       </c>
       <c r="B46" t="s">
@@ -3670,7 +3851,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" t="s">
+      <c r="A47" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B47" t="s">
@@ -3697,7 +3878,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" t="s">
+      <c r="A48" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B48" t="s">
@@ -3739,7 +3920,7 @@
       <c r="E49" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="10" t="s">
         <v>336</v>
       </c>
       <c r="G49" t="str">
@@ -3751,7 +3932,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" t="s">
+      <c r="A50" s="33" t="s">
         <v>69</v>
       </c>
       <c r="B50" t="s">
@@ -3832,7 +4013,7 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" t="s">
+      <c r="A53" s="33" t="s">
         <v>70</v>
       </c>
       <c r="B53" t="s">
@@ -3859,7 +4040,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" t="s">
+      <c r="A54" s="33" t="s">
         <v>71</v>
       </c>
       <c r="B54" t="s">
@@ -3940,7 +4121,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" t="s">
+      <c r="A57" s="33" t="s">
         <v>74</v>
       </c>
       <c r="B57" t="s">
@@ -3964,7 +4145,7 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" t="s">
+      <c r="A58" s="33" t="s">
         <v>75</v>
       </c>
       <c r="B58" t="s">
@@ -6258,255 +6439,719 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5775640E-8023-4E82-86E7-18CF3F672339}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:46">
+      <c r="A1" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:46">
+      <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="33" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2260668</v>
+      </c>
+      <c r="U2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AT2" s="34"/>
+    </row>
+    <row r="3" spans="1:46">
+      <c r="A3" s="32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="34" t="s">
+      <c r="B3">
+        <v>2260668</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="34" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46">
+      <c r="A5" s="33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="34" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>10057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46">
+      <c r="A6" s="33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="34" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46">
+      <c r="A7" s="33" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="34" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46">
+      <c r="A8" s="33" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="34" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>93301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46">
+      <c r="A9" s="33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="34" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46">
+      <c r="A10" s="33" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="34" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46">
+      <c r="A11" s="33" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="34" t="s">
+      <c r="B11">
+        <v>166969</v>
+      </c>
+      <c r="C11">
+        <v>7.3858300000000002E-2</v>
+      </c>
+      <c r="D11">
+        <v>512694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46">
+      <c r="A12" s="33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="34" t="s">
+      <c r="B12">
+        <v>146907</v>
+      </c>
+      <c r="C12">
+        <v>6.4983899999999997E-2</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46">
+      <c r="A13" s="33" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="34" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46">
+      <c r="A14" s="33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="34" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1.7999999999999999E-6</v>
+      </c>
+      <c r="D14">
+        <v>89369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46">
+      <c r="A15" s="33" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="34" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46">
+      <c r="A16" s="33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="34" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="34" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="34" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="34">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D18">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="34" t="s">
+      <c r="B19">
+        <v>23326</v>
+      </c>
+      <c r="C19">
+        <v>1.03182E-2</v>
+      </c>
+      <c r="D19" s="34">
+        <v>63168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="34" t="s">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="34">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="D20" s="34">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="34" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D21">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="34" t="s">
+      <c r="B22">
+        <v>1712</v>
+      </c>
+      <c r="C22">
+        <v>7.5730000000000003E-4</v>
+      </c>
+      <c r="D22">
+        <v>11051</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="34" t="s">
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>1.33E-5</v>
+      </c>
+      <c r="D23">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="34" t="s">
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>1.33E-5</v>
+      </c>
+      <c r="D24" s="34">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="34" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="34">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D25" s="34">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="34" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="34">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D26">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="34" t="s">
+      <c r="B27">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>1.3699999999999999E-5</v>
+      </c>
+      <c r="D27">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="34" t="s">
+      <c r="B28">
+        <v>1158341</v>
+      </c>
+      <c r="C28">
+        <v>0.51238879999999998</v>
+      </c>
+      <c r="D28">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="34" t="s">
+      <c r="B29">
+        <v>1901321</v>
+      </c>
+      <c r="C29">
+        <v>0.84104389999999996</v>
+      </c>
+      <c r="D29">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="34" t="s">
+      <c r="B30">
+        <v>110</v>
+      </c>
+      <c r="C30">
+        <v>4.8699999999999998E-5</v>
+      </c>
+      <c r="D30">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="34" t="s">
+      <c r="B31">
+        <v>92</v>
+      </c>
+      <c r="C31">
+        <v>4.07E-5</v>
+      </c>
+      <c r="D31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="33" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="34" t="s">
+      <c r="B32">
+        <v>54</v>
+      </c>
+      <c r="C32">
+        <v>2.3900000000000002E-5</v>
+      </c>
+      <c r="D32">
+        <v>102286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="34" t="s">
+      <c r="B33">
+        <v>1834</v>
+      </c>
+      <c r="C33">
+        <v>8.1130000000000004E-4</v>
+      </c>
+      <c r="D33">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="34" t="s">
+      <c r="B34">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>2.2099999999999998E-5</v>
+      </c>
+      <c r="D34">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="34" t="s">
+      <c r="B35">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>7.5000000000000002E-6</v>
+      </c>
+      <c r="D35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="33" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="34" t="s">
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>7.5000000000000002E-6</v>
+      </c>
+      <c r="D36">
+        <v>356239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="33" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="34" t="s">
+      <c r="B37">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>9.3000000000000007E-6</v>
+      </c>
+      <c r="D37">
+        <v>368550</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="34" t="s">
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>5.8000000000000004E-6</v>
+      </c>
+      <c r="D38">
+        <v>1633693</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="33" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="34" t="s">
+      <c r="B39">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>4.8999999999999997E-6</v>
+      </c>
+      <c r="D39">
+        <v>1311060</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="34" t="s">
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="D40">
+        <v>486576</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="33" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="34" t="s">
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>1.3E-6</v>
+      </c>
+      <c r="D41">
+        <v>636000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="33" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="34" t="s">
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>1.3E-6</v>
+      </c>
+      <c r="D42" s="34">
+        <v>18530</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="33" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="34" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" s="34">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="D43">
+        <v>132850</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="33" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="34" t="s">
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>2.7E-6</v>
+      </c>
+      <c r="D44">
+        <v>146314</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="33" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="34" t="s">
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>1.3E-6</v>
+      </c>
+      <c r="D45">
+        <v>704487</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="33" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="34" t="s">
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <v>1.9000000000000001E-5</v>
+      </c>
+      <c r="D46">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="34" t="s">
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>1.5500000000000001E-5</v>
+      </c>
+      <c r="D47">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="33" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="34" t="s">
+      <c r="B48">
+        <v>66</v>
+      </c>
+      <c r="C48">
+        <v>2.9200000000000002E-5</v>
+      </c>
+      <c r="D48">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="33" t="s">
         <v>75</v>
+      </c>
+      <c r="B49">
+        <v>55</v>
+      </c>
+      <c r="C49">
+        <v>2.4300000000000001E-5</v>
+      </c>
+      <c r="D49">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6532,185 +7177,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="31.9">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.65" thickBot="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="28.5">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>347</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="57">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>20</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="57">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>350</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>18</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="57">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>12</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="57">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>15</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="42.75">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>357</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>8</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="42.75">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>8</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="42.75">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>362</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>6</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="42.75">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>5</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="42.75">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>369</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="14.65" thickBot="1">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="27">
+      <c r="B15" s="25"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="26">
         <v>100</v>
       </c>
       <c r="E15" s="1"/>
@@ -6723,15 +7368,15 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.5">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>374</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -6742,7 +7387,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>375</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -6753,7 +7398,7 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>379</v>
       </c>
       <c r="B20" t="s">
@@ -6832,7 +7477,7 @@
         <v>66</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="14"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
@@ -6918,8 +7563,8 @@
       <c r="A1" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -6927,6 +7572,563 @@
       </c>
       <c r="B2" t="s">
         <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0259719E-8A60-4BBE-A5F9-5A66971B39D0}">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="21.265625" customWidth="1"/>
+    <col min="2" max="2" width="50.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated null percentages after replacing malformed values with null
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\lending_club_credit_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26785EE3-1B24-4A0D-A124-497E81726C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED96C4F8-9CAB-4FDA-817F-DD7373C0AF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{E942A053-C755-425D-9049-8D107678D16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns_description" sheetId="1" r:id="rId1"/>
@@ -2119,7 +2119,7 @@
     <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2198,16 +2198,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2605,7 +2598,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.59765625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="33.59765625" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
     <col min="3" max="3" width="18.19921875" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
@@ -2615,7 +2608,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -2641,7 +2634,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2660,7 +2653,7 @@
         <v>52</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(ISNUMBER(MATCH(A2, H:H, 0)), "Y", "N")</f>
+        <f t="shared" ref="G2:G33" si="0">IF(ISNUMBER(MATCH(A2, H:H, 0)), "Y", "N")</f>
         <v>Y</v>
       </c>
       <c r="H2" t="s">
@@ -2668,7 +2661,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1"/>
@@ -2685,7 +2678,7 @@
         <v>53</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(ISNUMBER(MATCH(A3, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H3" t="s">
@@ -2712,7 +2705,7 @@
         <v>16</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(ISNUMBER(MATCH(A4, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>N</v>
       </c>
       <c r="H4" t="s">
@@ -2720,10 +2713,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="33" t="s">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2739,7 +2732,7 @@
         <v>201</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(ISNUMBER(MATCH(A5, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H5" t="s">
@@ -2747,10 +2740,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="33" t="s">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2766,7 +2759,7 @@
         <v>201</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(ISNUMBER(MATCH(A6, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H6" t="s">
@@ -2774,7 +2767,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="33" t="s">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -2793,7 +2786,7 @@
         <v>339</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(ISNUMBER(MATCH(A7, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H7" t="s">
@@ -2801,7 +2794,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="33" t="s">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -2820,7 +2813,7 @@
         <v>172</v>
       </c>
       <c r="G8" t="str">
-        <f>IF(ISNUMBER(MATCH(A8, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H8" t="s">
@@ -2828,7 +2821,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="33" t="s">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2847,7 +2840,7 @@
         <v>174</v>
       </c>
       <c r="G9" t="str">
-        <f>IF(ISNUMBER(MATCH(A9, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H9" t="s">
@@ -2855,7 +2848,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="33" t="s">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2874,7 +2867,7 @@
         <v>176</v>
       </c>
       <c r="G10" t="str">
-        <f>IF(ISNUMBER(MATCH(A10, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H10" t="s">
@@ -2882,7 +2875,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="33" t="s">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2901,7 +2894,7 @@
         <v>178</v>
       </c>
       <c r="G11" t="str">
-        <f>IF(ISNUMBER(MATCH(A11, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H11" t="s">
@@ -2909,7 +2902,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="33" t="s">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2928,7 +2921,7 @@
         <v>185</v>
       </c>
       <c r="G12" t="str">
-        <f>IF(ISNUMBER(MATCH(A12, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H12" t="s">
@@ -2936,7 +2929,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="33" t="s">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2955,7 +2948,7 @@
         <v>181</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(ISNUMBER(MATCH(A13, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H13" t="s">
@@ -2963,7 +2956,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="33" t="s">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2982,7 +2975,7 @@
         <v>186</v>
       </c>
       <c r="G14" t="str">
-        <f>IF(ISNUMBER(MATCH(A14, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H14" t="s">
@@ -2990,7 +2983,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="33" t="s">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3009,7 +3002,7 @@
         <v>187</v>
       </c>
       <c r="G15" t="str">
-        <f>IF(ISNUMBER(MATCH(A15, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H15" t="s">
@@ -3017,7 +3010,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="33" t="s">
+      <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16" t="s">
@@ -3036,7 +3029,7 @@
         <v>189</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(ISNUMBER(MATCH(A16, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H16" t="s">
@@ -3044,7 +3037,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="33" t="s">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -3063,7 +3056,7 @@
         <v>192</v>
       </c>
       <c r="G17" t="str">
-        <f>IF(ISNUMBER(MATCH(A17, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H17" t="s">
@@ -3071,7 +3064,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="33" t="s">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3090,7 +3083,7 @@
         <v>194</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(ISNUMBER(MATCH(A18, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H18" t="s">
@@ -3117,7 +3110,7 @@
         <v>197</v>
       </c>
       <c r="G19" t="str">
-        <f>IF(ISNUMBER(MATCH(A19, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>N</v>
       </c>
       <c r="H19" t="s">
@@ -3144,7 +3137,7 @@
         <v>199</v>
       </c>
       <c r="G20" t="str">
-        <f>IF(ISNUMBER(MATCH(A20, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>N</v>
       </c>
       <c r="H20" t="s">
@@ -3168,7 +3161,7 @@
         <v>199</v>
       </c>
       <c r="G21" t="str">
-        <f>IF(ISNUMBER(MATCH(A21, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>N</v>
       </c>
       <c r="H21" t="s">
@@ -3176,7 +3169,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="33" t="s">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
@@ -3195,7 +3188,7 @@
         <v>201</v>
       </c>
       <c r="G22" t="str">
-        <f>IF(ISNUMBER(MATCH(A22, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H22" t="s">
@@ -3203,7 +3196,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="33" t="s">
+      <c r="A23" t="s">
         <v>58</v>
       </c>
       <c r="B23" t="s">
@@ -3222,7 +3215,7 @@
         <v>202</v>
       </c>
       <c r="G23" t="str">
-        <f>IF(ISNUMBER(MATCH(A23, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H23" t="s">
@@ -3230,7 +3223,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="33" t="s">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
       <c r="B24" t="s">
@@ -3249,7 +3242,7 @@
         <v>201</v>
       </c>
       <c r="G24" t="str">
-        <f>IF(ISNUMBER(MATCH(A24, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H24" t="s">
@@ -3257,7 +3250,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="33" t="s">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
@@ -3276,7 +3269,7 @@
         <v>201</v>
       </c>
       <c r="G25" t="str">
-        <f>IF(ISNUMBER(MATCH(A25, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H25" t="s">
@@ -3284,10 +3277,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.5">
-      <c r="A26" s="33" t="s">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="33" t="s">
         <v>341</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -3303,7 +3296,7 @@
         <v>205</v>
       </c>
       <c r="G26" t="str">
-        <f>IF(ISNUMBER(MATCH(A26, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H26" t="s">
@@ -3311,7 +3304,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="33" t="s">
+      <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
@@ -3330,7 +3323,7 @@
         <v>201</v>
       </c>
       <c r="G27" t="str">
-        <f>IF(ISNUMBER(MATCH(A27, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H27" t="s">
@@ -3338,7 +3331,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="33" t="s">
+      <c r="A28" t="s">
         <v>60</v>
       </c>
       <c r="B28" t="s">
@@ -3357,7 +3350,7 @@
         <v>201</v>
       </c>
       <c r="G28" t="str">
-        <f>IF(ISNUMBER(MATCH(A28, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H28" t="s">
@@ -3365,7 +3358,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="33" t="s">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
@@ -3384,7 +3377,7 @@
         <v>201</v>
       </c>
       <c r="G29" t="str">
-        <f>IF(ISNUMBER(MATCH(A29, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H29" t="s">
@@ -3392,7 +3385,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="33" t="s">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
       <c r="B30" t="s">
@@ -3411,7 +3404,7 @@
         <v>201</v>
       </c>
       <c r="G30" t="str">
-        <f>IF(ISNUMBER(MATCH(A30, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H30" t="s">
@@ -3419,7 +3412,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="33" t="s">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
       <c r="B31" t="s">
@@ -3438,7 +3431,7 @@
         <v>201</v>
       </c>
       <c r="G31" t="str">
-        <f>IF(ISNUMBER(MATCH(A31, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H31" t="s">
@@ -3446,7 +3439,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="33" t="s">
+      <c r="A32" t="s">
         <v>62</v>
       </c>
       <c r="B32" t="s">
@@ -3465,7 +3458,7 @@
         <v>201</v>
       </c>
       <c r="G32" t="str">
-        <f>IF(ISNUMBER(MATCH(A32, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H32" t="s">
@@ -3473,10 +3466,10 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="33" t="s">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="33" t="s">
         <v>214</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -3492,7 +3485,7 @@
         <v>201</v>
       </c>
       <c r="G33" t="str">
-        <f>IF(ISNUMBER(MATCH(A33, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="0"/>
         <v>Y</v>
       </c>
       <c r="H33" t="s">
@@ -3500,7 +3493,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="33" t="s">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
@@ -3519,7 +3512,7 @@
         <v>201</v>
       </c>
       <c r="G34" t="str">
-        <f>IF(ISNUMBER(MATCH(A34, H:H, 0)), "Y", "N")</f>
+        <f t="shared" ref="G34:G65" si="1">IF(ISNUMBER(MATCH(A34, H:H, 0)), "Y", "N")</f>
         <v>Y</v>
       </c>
       <c r="H34" t="s">
@@ -3527,7 +3520,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="33" t="s">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
@@ -3546,7 +3539,7 @@
         <v>201</v>
       </c>
       <c r="G35" t="str">
-        <f>IF(ISNUMBER(MATCH(A35, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H35" t="s">
@@ -3554,7 +3547,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="33" t="s">
+      <c r="A36" t="s">
         <v>64</v>
       </c>
       <c r="B36" t="s">
@@ -3573,7 +3566,7 @@
         <v>216</v>
       </c>
       <c r="G36" t="str">
-        <f>IF(ISNUMBER(MATCH(A36, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H36" t="s">
@@ -3581,7 +3574,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="28.5">
-      <c r="A37" s="33" t="s">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
       <c r="B37" t="s">
@@ -3600,7 +3593,7 @@
         <v>217</v>
       </c>
       <c r="G37" t="str">
-        <f>IF(ISNUMBER(MATCH(A37, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H37" t="s">
@@ -3608,7 +3601,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="33" t="s">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -3627,7 +3620,7 @@
         <v>219</v>
       </c>
       <c r="G38" t="str">
-        <f>IF(ISNUMBER(MATCH(A38, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H38" t="s">
@@ -3635,7 +3628,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="33" t="s">
+      <c r="A39" t="s">
         <v>65</v>
       </c>
       <c r="B39" t="s">
@@ -3654,7 +3647,7 @@
         <v>201</v>
       </c>
       <c r="G39" t="str">
-        <f>IF(ISNUMBER(MATCH(A39, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H39" t="s">
@@ -3662,7 +3655,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="33" t="s">
+      <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
@@ -3681,7 +3674,7 @@
         <v>201</v>
       </c>
       <c r="G40" t="str">
-        <f>IF(ISNUMBER(MATCH(A40, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H40" t="s">
@@ -3689,7 +3682,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="33" t="s">
+      <c r="A41" t="s">
         <v>66</v>
       </c>
       <c r="B41" t="s">
@@ -3708,7 +3701,7 @@
         <v>201</v>
       </c>
       <c r="G41" t="str">
-        <f>IF(ISNUMBER(MATCH(A41, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H41" t="s">
@@ -3716,7 +3709,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="33" t="s">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
       <c r="B42" t="s">
@@ -3735,7 +3728,7 @@
         <v>342</v>
       </c>
       <c r="G42" t="str">
-        <f>IF(ISNUMBER(MATCH(A42, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H42" t="s">
@@ -3743,7 +3736,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="33" t="s">
+      <c r="A43" t="s">
         <v>67</v>
       </c>
       <c r="B43" t="s">
@@ -3762,7 +3755,7 @@
         <v>201</v>
       </c>
       <c r="G43" t="str">
-        <f>IF(ISNUMBER(MATCH(A43, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H43" t="s">
@@ -3770,7 +3763,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="33" t="s">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
@@ -3789,7 +3782,7 @@
         <v>201</v>
       </c>
       <c r="G44" t="str">
-        <f>IF(ISNUMBER(MATCH(A44, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H44" t="s">
@@ -3797,7 +3790,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="33" t="s">
+      <c r="A45" t="s">
         <v>41</v>
       </c>
       <c r="B45" t="s">
@@ -3816,7 +3809,7 @@
         <v>201</v>
       </c>
       <c r="G45" t="str">
-        <f>IF(ISNUMBER(MATCH(A45, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H45" t="s">
@@ -3824,7 +3817,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="33" t="s">
+      <c r="A46" t="s">
         <v>68</v>
       </c>
       <c r="B46" t="s">
@@ -3843,7 +3836,7 @@
         <v>201</v>
       </c>
       <c r="G46" t="str">
-        <f>IF(ISNUMBER(MATCH(A46, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H46" t="s">
@@ -3851,7 +3844,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="33" t="s">
+      <c r="A47" t="s">
         <v>42</v>
       </c>
       <c r="B47" t="s">
@@ -3870,7 +3863,7 @@
         <v>201</v>
       </c>
       <c r="G47" t="str">
-        <f>IF(ISNUMBER(MATCH(A47, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H47" t="s">
@@ -3878,7 +3871,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="33" t="s">
+      <c r="A48" t="s">
         <v>43</v>
       </c>
       <c r="B48" t="s">
@@ -3897,7 +3890,7 @@
         <v>201</v>
       </c>
       <c r="G48" t="str">
-        <f>IF(ISNUMBER(MATCH(A48, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H48" t="s">
@@ -3924,7 +3917,7 @@
         <v>336</v>
       </c>
       <c r="G49" t="str">
-        <f>IF(ISNUMBER(MATCH(A49, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="H49" t="s">
@@ -3932,7 +3925,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="33" t="s">
+      <c r="A50" t="s">
         <v>69</v>
       </c>
       <c r="B50" t="s">
@@ -3951,7 +3944,7 @@
         <v>201</v>
       </c>
       <c r="G50" t="str">
-        <f>IF(ISNUMBER(MATCH(A50, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H50" t="s">
@@ -3978,7 +3971,7 @@
         <v>201</v>
       </c>
       <c r="G51" t="str">
-        <f>IF(ISNUMBER(MATCH(A51, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="H51" t="s">
@@ -4005,7 +3998,7 @@
         <v>201</v>
       </c>
       <c r="G52" t="str">
-        <f>IF(ISNUMBER(MATCH(A52, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="H52" t="s">
@@ -4013,7 +4006,7 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="33" t="s">
+      <c r="A53" t="s">
         <v>70</v>
       </c>
       <c r="B53" t="s">
@@ -4032,7 +4025,7 @@
         <v>201</v>
       </c>
       <c r="G53" t="str">
-        <f>IF(ISNUMBER(MATCH(A53, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H53" t="s">
@@ -4040,7 +4033,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="33" t="s">
+      <c r="A54" t="s">
         <v>71</v>
       </c>
       <c r="B54" t="s">
@@ -4059,7 +4052,7 @@
         <v>201</v>
       </c>
       <c r="G54" t="str">
-        <f>IF(ISNUMBER(MATCH(A54, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
       <c r="H54" t="s">
@@ -4086,7 +4079,7 @@
         <v>201</v>
       </c>
       <c r="G55" t="str">
-        <f>IF(ISNUMBER(MATCH(A55, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="H55" t="s">
@@ -4113,7 +4106,7 @@
         <v>337</v>
       </c>
       <c r="G56" t="str">
-        <f>IF(ISNUMBER(MATCH(A56, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
       <c r="H56" t="s">
@@ -4121,7 +4114,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="33" t="s">
+      <c r="A57" t="s">
         <v>74</v>
       </c>
       <c r="B57" t="s">
@@ -4140,12 +4133,12 @@
         <v>201</v>
       </c>
       <c r="G57" t="str">
-        <f>IF(ISNUMBER(MATCH(A57, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="33" t="s">
+      <c r="A58" t="s">
         <v>75</v>
       </c>
       <c r="B58" t="s">
@@ -4164,7 +4157,7 @@
         <v>201</v>
       </c>
       <c r="G58" t="str">
-        <f>IF(ISNUMBER(MATCH(A58, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>Y</v>
       </c>
     </row>
@@ -4188,7 +4181,7 @@
         <v>201</v>
       </c>
       <c r="G59" t="str">
-        <f>IF(ISNUMBER(MATCH(A59, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4212,7 +4205,7 @@
         <v>201</v>
       </c>
       <c r="G60" t="str">
-        <f>IF(ISNUMBER(MATCH(A60, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4236,7 +4229,7 @@
         <v>201</v>
       </c>
       <c r="G61" t="str">
-        <f>IF(ISNUMBER(MATCH(A61, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4260,7 +4253,7 @@
         <v>201</v>
       </c>
       <c r="G62" t="str">
-        <f>IF(ISNUMBER(MATCH(A62, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4284,7 +4277,7 @@
         <v>201</v>
       </c>
       <c r="G63" t="str">
-        <f>IF(ISNUMBER(MATCH(A63, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4308,7 +4301,7 @@
         <v>201</v>
       </c>
       <c r="G64" t="str">
-        <f>IF(ISNUMBER(MATCH(A64, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4332,7 +4325,7 @@
         <v>201</v>
       </c>
       <c r="G65" t="str">
-        <f>IF(ISNUMBER(MATCH(A65, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="1"/>
         <v>N</v>
       </c>
     </row>
@@ -4356,7 +4349,7 @@
         <v>201</v>
       </c>
       <c r="G66" t="str">
-        <f>IF(ISNUMBER(MATCH(A66, H:H, 0)), "Y", "N")</f>
+        <f t="shared" ref="G66:G97" si="2">IF(ISNUMBER(MATCH(A66, H:H, 0)), "Y", "N")</f>
         <v>N</v>
       </c>
     </row>
@@ -4380,7 +4373,7 @@
         <v>201</v>
       </c>
       <c r="G67" t="str">
-        <f>IF(ISNUMBER(MATCH(A67, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4404,7 +4397,7 @@
         <v>201</v>
       </c>
       <c r="G68" t="str">
-        <f>IF(ISNUMBER(MATCH(A68, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4428,7 +4421,7 @@
         <v>201</v>
       </c>
       <c r="G69" t="str">
-        <f>IF(ISNUMBER(MATCH(A69, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4452,7 +4445,7 @@
         <v>201</v>
       </c>
       <c r="G70" t="str">
-        <f>IF(ISNUMBER(MATCH(A70, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4476,7 +4469,7 @@
         <v>333</v>
       </c>
       <c r="G71" t="str">
-        <f>IF(ISNUMBER(MATCH(A71, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4500,7 +4493,7 @@
         <v>201</v>
       </c>
       <c r="G72" t="str">
-        <f>IF(ISNUMBER(MATCH(A72, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4524,7 +4517,7 @@
         <v>201</v>
       </c>
       <c r="G73" t="str">
-        <f>IF(ISNUMBER(MATCH(A73, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4548,7 +4541,7 @@
         <v>334</v>
       </c>
       <c r="G74" t="str">
-        <f>IF(ISNUMBER(MATCH(A74, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4572,7 +4565,7 @@
         <v>201</v>
       </c>
       <c r="G75" t="str">
-        <f>IF(ISNUMBER(MATCH(A75, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4596,7 +4589,7 @@
         <v>334</v>
       </c>
       <c r="G76" t="str">
-        <f>IF(ISNUMBER(MATCH(A76, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4620,7 +4613,7 @@
         <v>201</v>
       </c>
       <c r="G77" t="str">
-        <f>IF(ISNUMBER(MATCH(A77, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4644,7 +4637,7 @@
         <v>201</v>
       </c>
       <c r="G78" t="str">
-        <f>IF(ISNUMBER(MATCH(A78, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4668,7 +4661,7 @@
         <v>201</v>
       </c>
       <c r="G79" t="str">
-        <f>IF(ISNUMBER(MATCH(A79, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4692,7 +4685,7 @@
         <v>201</v>
       </c>
       <c r="G80" t="str">
-        <f>IF(ISNUMBER(MATCH(A80, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4716,7 +4709,7 @@
         <v>201</v>
       </c>
       <c r="G81" t="str">
-        <f>IF(ISNUMBER(MATCH(A81, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4740,7 +4733,7 @@
         <v>201</v>
       </c>
       <c r="G82" t="str">
-        <f>IF(ISNUMBER(MATCH(A82, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4764,7 +4757,7 @@
         <v>201</v>
       </c>
       <c r="G83" t="str">
-        <f>IF(ISNUMBER(MATCH(A83, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4788,7 +4781,7 @@
         <v>201</v>
       </c>
       <c r="G84" t="str">
-        <f>IF(ISNUMBER(MATCH(A84, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4812,7 +4805,7 @@
         <v>201</v>
       </c>
       <c r="G85" t="str">
-        <f>IF(ISNUMBER(MATCH(A85, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4836,7 +4829,7 @@
         <v>201</v>
       </c>
       <c r="G86" t="str">
-        <f>IF(ISNUMBER(MATCH(A86, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4860,7 +4853,7 @@
         <v>201</v>
       </c>
       <c r="G87" t="str">
-        <f>IF(ISNUMBER(MATCH(A87, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4884,7 +4877,7 @@
         <v>201</v>
       </c>
       <c r="G88" t="str">
-        <f>IF(ISNUMBER(MATCH(A88, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4908,7 +4901,7 @@
         <v>201</v>
       </c>
       <c r="G89" t="str">
-        <f>IF(ISNUMBER(MATCH(A89, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4932,7 +4925,7 @@
         <v>201</v>
       </c>
       <c r="G90" t="str">
-        <f>IF(ISNUMBER(MATCH(A90, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4956,7 +4949,7 @@
         <v>201</v>
       </c>
       <c r="G91" t="str">
-        <f>IF(ISNUMBER(MATCH(A91, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -4980,7 +4973,7 @@
         <v>201</v>
       </c>
       <c r="G92" t="str">
-        <f>IF(ISNUMBER(MATCH(A92, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5004,7 +4997,7 @@
         <v>201</v>
       </c>
       <c r="G93" t="str">
-        <f>IF(ISNUMBER(MATCH(A93, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5028,7 +5021,7 @@
         <v>201</v>
       </c>
       <c r="G94" t="str">
-        <f>IF(ISNUMBER(MATCH(A94, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5052,7 +5045,7 @@
         <v>201</v>
       </c>
       <c r="G95" t="str">
-        <f>IF(ISNUMBER(MATCH(A95, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5076,7 +5069,7 @@
         <v>201</v>
       </c>
       <c r="G96" t="str">
-        <f>IF(ISNUMBER(MATCH(A96, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5100,7 +5093,7 @@
         <v>201</v>
       </c>
       <c r="G97" t="str">
-        <f>IF(ISNUMBER(MATCH(A97, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="2"/>
         <v>N</v>
       </c>
     </row>
@@ -5124,7 +5117,7 @@
         <v>201</v>
       </c>
       <c r="G98" t="str">
-        <f>IF(ISNUMBER(MATCH(A98, H:H, 0)), "Y", "N")</f>
+        <f t="shared" ref="G98:G129" si="3">IF(ISNUMBER(MATCH(A98, H:H, 0)), "Y", "N")</f>
         <v>N</v>
       </c>
     </row>
@@ -5148,7 +5141,7 @@
         <v>201</v>
       </c>
       <c r="G99" t="str">
-        <f>IF(ISNUMBER(MATCH(A99, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5172,7 +5165,7 @@
         <v>201</v>
       </c>
       <c r="G100" t="str">
-        <f>IF(ISNUMBER(MATCH(A100, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5196,7 +5189,7 @@
         <v>201</v>
       </c>
       <c r="G101" t="str">
-        <f>IF(ISNUMBER(MATCH(A101, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5220,7 +5213,7 @@
         <v>201</v>
       </c>
       <c r="G102" t="str">
-        <f>IF(ISNUMBER(MATCH(A102, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5244,7 +5237,7 @@
         <v>201</v>
       </c>
       <c r="G103" t="str">
-        <f>IF(ISNUMBER(MATCH(A103, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5268,7 +5261,7 @@
         <v>201</v>
       </c>
       <c r="G104" t="str">
-        <f>IF(ISNUMBER(MATCH(A104, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5292,7 +5285,7 @@
         <v>201</v>
       </c>
       <c r="G105" t="str">
-        <f>IF(ISNUMBER(MATCH(A105, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5316,7 +5309,7 @@
         <v>201</v>
       </c>
       <c r="G106" t="str">
-        <f>IF(ISNUMBER(MATCH(A106, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5340,7 +5333,7 @@
         <v>201</v>
       </c>
       <c r="G107" t="str">
-        <f>IF(ISNUMBER(MATCH(A107, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5364,7 +5357,7 @@
         <v>201</v>
       </c>
       <c r="G108" t="str">
-        <f>IF(ISNUMBER(MATCH(A108, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5388,7 +5381,7 @@
         <v>201</v>
       </c>
       <c r="G109" t="str">
-        <f>IF(ISNUMBER(MATCH(A109, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5412,7 +5405,7 @@
         <v>201</v>
       </c>
       <c r="G110" t="str">
-        <f>IF(ISNUMBER(MATCH(A110, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5436,7 +5429,7 @@
         <v>201</v>
       </c>
       <c r="G111" t="str">
-        <f>IF(ISNUMBER(MATCH(A111, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5460,7 +5453,7 @@
         <v>201</v>
       </c>
       <c r="G112" t="str">
-        <f>IF(ISNUMBER(MATCH(A112, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5484,7 +5477,7 @@
         <v>201</v>
       </c>
       <c r="G113" t="str">
-        <f>IF(ISNUMBER(MATCH(A113, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5508,7 +5501,7 @@
         <v>201</v>
       </c>
       <c r="G114" t="str">
-        <f>IF(ISNUMBER(MATCH(A114, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5532,7 +5525,7 @@
         <v>201</v>
       </c>
       <c r="G115" t="str">
-        <f>IF(ISNUMBER(MATCH(A115, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5556,7 +5549,7 @@
         <v>201</v>
       </c>
       <c r="G116" t="str">
-        <f>IF(ISNUMBER(MATCH(A116, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5580,7 +5573,7 @@
         <v>53</v>
       </c>
       <c r="G117" t="str">
-        <f>IF(ISNUMBER(MATCH(A117, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5604,7 +5597,7 @@
         <v>53</v>
       </c>
       <c r="G118" t="str">
-        <f>IF(ISNUMBER(MATCH(A118, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5628,7 +5621,7 @@
         <v>53</v>
       </c>
       <c r="G119" t="str">
-        <f>IF(ISNUMBER(MATCH(A119, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5652,7 +5645,7 @@
         <v>53</v>
       </c>
       <c r="G120" t="str">
-        <f>IF(ISNUMBER(MATCH(A120, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5676,7 +5669,7 @@
         <v>53</v>
       </c>
       <c r="G121" t="str">
-        <f>IF(ISNUMBER(MATCH(A121, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5700,7 +5693,7 @@
         <v>53</v>
       </c>
       <c r="G122" t="str">
-        <f>IF(ISNUMBER(MATCH(A122, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5724,7 +5717,7 @@
         <v>53</v>
       </c>
       <c r="G123" t="str">
-        <f>IF(ISNUMBER(MATCH(A123, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5748,7 +5741,7 @@
         <v>53</v>
       </c>
       <c r="G124" t="str">
-        <f>IF(ISNUMBER(MATCH(A124, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5772,7 +5765,7 @@
         <v>53</v>
       </c>
       <c r="G125" t="str">
-        <f>IF(ISNUMBER(MATCH(A125, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5796,7 +5789,7 @@
         <v>53</v>
       </c>
       <c r="G126" t="str">
-        <f>IF(ISNUMBER(MATCH(A126, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5820,7 +5813,7 @@
         <v>53</v>
       </c>
       <c r="G127" t="str">
-        <f>IF(ISNUMBER(MATCH(A127, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5844,7 +5837,7 @@
         <v>53</v>
       </c>
       <c r="G128" t="str">
-        <f>IF(ISNUMBER(MATCH(A128, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5868,7 +5861,7 @@
         <v>53</v>
       </c>
       <c r="G129" t="str">
-        <f>IF(ISNUMBER(MATCH(A129, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="3"/>
         <v>N</v>
       </c>
     </row>
@@ -5892,7 +5885,7 @@
         <v>53</v>
       </c>
       <c r="G130" t="str">
-        <f>IF(ISNUMBER(MATCH(A130, H:H, 0)), "Y", "N")</f>
+        <f t="shared" ref="G130:G161" si="4">IF(ISNUMBER(MATCH(A130, H:H, 0)), "Y", "N")</f>
         <v>N</v>
       </c>
     </row>
@@ -5916,7 +5909,7 @@
         <v>53</v>
       </c>
       <c r="G131" t="str">
-        <f>IF(ISNUMBER(MATCH(A131, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -5940,7 +5933,7 @@
         <v>53</v>
       </c>
       <c r="G132" t="str">
-        <f>IF(ISNUMBER(MATCH(A132, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -5964,7 +5957,7 @@
         <v>53</v>
       </c>
       <c r="G133" t="str">
-        <f>IF(ISNUMBER(MATCH(A133, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -5988,7 +5981,7 @@
         <v>53</v>
       </c>
       <c r="G134" t="str">
-        <f>IF(ISNUMBER(MATCH(A134, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6012,7 +6005,7 @@
         <v>53</v>
       </c>
       <c r="G135" t="str">
-        <f>IF(ISNUMBER(MATCH(A135, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6036,7 +6029,7 @@
         <v>53</v>
       </c>
       <c r="G136" t="str">
-        <f>IF(ISNUMBER(MATCH(A136, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6060,7 +6053,7 @@
         <v>53</v>
       </c>
       <c r="G137" t="str">
-        <f>IF(ISNUMBER(MATCH(A137, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6084,7 +6077,7 @@
         <v>53</v>
       </c>
       <c r="G138" t="str">
-        <f>IF(ISNUMBER(MATCH(A138, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6108,7 +6101,7 @@
         <v>53</v>
       </c>
       <c r="G139" t="str">
-        <f>IF(ISNUMBER(MATCH(A139, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6132,7 +6125,7 @@
         <v>53</v>
       </c>
       <c r="G140" t="str">
-        <f>IF(ISNUMBER(MATCH(A140, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6156,7 +6149,7 @@
         <v>53</v>
       </c>
       <c r="G141" t="str">
-        <f>IF(ISNUMBER(MATCH(A141, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6180,7 +6173,7 @@
         <v>53</v>
       </c>
       <c r="G142" t="str">
-        <f>IF(ISNUMBER(MATCH(A142, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6204,7 +6197,7 @@
         <v>53</v>
       </c>
       <c r="G143" t="str">
-        <f>IF(ISNUMBER(MATCH(A143, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6228,7 +6221,7 @@
         <v>53</v>
       </c>
       <c r="G144" t="str">
-        <f>IF(ISNUMBER(MATCH(A144, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6252,7 +6245,7 @@
         <v>53</v>
       </c>
       <c r="G145" t="str">
-        <f>IF(ISNUMBER(MATCH(A145, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6276,7 +6269,7 @@
         <v>53</v>
       </c>
       <c r="G146" t="str">
-        <f>IF(ISNUMBER(MATCH(A146, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6300,7 +6293,7 @@
         <v>53</v>
       </c>
       <c r="G147" t="str">
-        <f>IF(ISNUMBER(MATCH(A147, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6324,7 +6317,7 @@
         <v>53</v>
       </c>
       <c r="G148" t="str">
-        <f>IF(ISNUMBER(MATCH(A148, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6348,7 +6341,7 @@
         <v>53</v>
       </c>
       <c r="G149" t="str">
-        <f>IF(ISNUMBER(MATCH(A149, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6372,7 +6365,7 @@
         <v>53</v>
       </c>
       <c r="G150" t="str">
-        <f>IF(ISNUMBER(MATCH(A150, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6396,7 +6389,7 @@
         <v>53</v>
       </c>
       <c r="G151" t="str">
-        <f>IF(ISNUMBER(MATCH(A151, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6420,7 +6413,7 @@
         <v>53</v>
       </c>
       <c r="G152" t="str">
-        <f>IF(ISNUMBER(MATCH(A152, H:H, 0)), "Y", "N")</f>
+        <f t="shared" si="4"/>
         <v>N</v>
       </c>
     </row>
@@ -6441,14 +6434,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5775640E-8023-4E82-86E7-18CF3F672339}">
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:BD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.19921875" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6477,7 +6470,7 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:46">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B2">
@@ -6489,15 +6482,15 @@
       <c r="D2">
         <v>2260668</v>
       </c>
-      <c r="U2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AT2" s="34"/>
+      <c r="U2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AT2" s="32"/>
     </row>
     <row r="3" spans="1:46">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3">
@@ -6511,7 +6504,7 @@
       </c>
     </row>
     <row r="4" spans="1:46">
-      <c r="A4" s="33" t="s">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4">
@@ -6525,7 +6518,7 @@
       </c>
     </row>
     <row r="5" spans="1:46">
-      <c r="A5" s="33" t="s">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5">
@@ -6539,7 +6532,7 @@
       </c>
     </row>
     <row r="6" spans="1:46">
-      <c r="A6" s="33" t="s">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
@@ -6553,7 +6546,7 @@
       </c>
     </row>
     <row r="7" spans="1:46">
-      <c r="A7" s="33" t="s">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
@@ -6567,7 +6560,7 @@
       </c>
     </row>
     <row r="8" spans="1:46">
-      <c r="A8" s="33" t="s">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8">
@@ -6581,7 +6574,7 @@
       </c>
     </row>
     <row r="9" spans="1:46">
-      <c r="A9" s="33" t="s">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
@@ -6593,9 +6586,13 @@
       <c r="D9">
         <v>7</v>
       </c>
+      <c r="W9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
     </row>
     <row r="10" spans="1:46">
-      <c r="A10" s="33" t="s">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
@@ -6609,7 +6606,7 @@
       </c>
     </row>
     <row r="11" spans="1:46">
-      <c r="A11" s="33" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11">
@@ -6623,7 +6620,7 @@
       </c>
     </row>
     <row r="12" spans="1:46">
-      <c r="A12" s="33" t="s">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12">
@@ -6637,7 +6634,7 @@
       </c>
     </row>
     <row r="13" spans="1:46">
-      <c r="A13" s="33" t="s">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13">
@@ -6651,21 +6648,21 @@
       </c>
     </row>
     <row r="14" spans="1:46">
-      <c r="A14" s="33" t="s">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>1.7999999999999999E-6</v>
+        <v>2.2000000000000001E-6</v>
       </c>
       <c r="D14">
         <v>89369</v>
       </c>
     </row>
     <row r="15" spans="1:46">
-      <c r="A15" s="33" t="s">
+      <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15">
@@ -6679,21 +6676,21 @@
       </c>
     </row>
     <row r="16" spans="1:46">
-      <c r="A16" s="33" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="32">
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="D16">
         <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="33" t="s">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17">
@@ -6702,18 +6699,18 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="33" t="s">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="32">
         <v>3.9999999999999998E-7</v>
       </c>
       <c r="D18">
@@ -6721,7 +6718,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="33" t="s">
+      <c r="A19" t="s">
         <v>58</v>
       </c>
       <c r="B19">
@@ -6730,32 +6727,32 @@
       <c r="C19">
         <v>1.03182E-2</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="32">
         <v>63168</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="33" t="s">
+      <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="32">
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="32">
         <v>1175</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="33" t="s">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>3.9999999999999998E-7</v>
       </c>
       <c r="D21">
@@ -6763,189 +6760,189 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="33" t="s">
+      <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22">
-        <v>1712</v>
+        <v>1967</v>
       </c>
       <c r="C22">
-        <v>7.5730000000000003E-4</v>
+        <v>8.7009999999999995E-4</v>
       </c>
       <c r="D22">
         <v>11051</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="33" t="s">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23">
-        <v>30</v>
+        <v>228</v>
       </c>
       <c r="C23">
-        <v>1.33E-5</v>
+        <v>1.009E-4</v>
       </c>
       <c r="D23">
         <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="33" t="s">
+      <c r="A24" t="s">
         <v>60</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>285</v>
       </c>
       <c r="C24">
-        <v>1.33E-5</v>
-      </c>
-      <c r="D24" s="34">
+        <v>1.261E-4</v>
+      </c>
+      <c r="D24" s="32">
         <v>926</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="33" t="s">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="34">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="D25" s="34">
+        <v>170</v>
+      </c>
+      <c r="C25">
+        <v>7.5199999999999998E-5</v>
+      </c>
+      <c r="D25" s="32">
         <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="33" t="s">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="34">
-        <v>3.9999999999999998E-7</v>
+        <v>137</v>
+      </c>
+      <c r="C26">
+        <v>6.0600000000000003E-5</v>
       </c>
       <c r="D26">
         <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="33" t="s">
+      <c r="A27" t="s">
         <v>61</v>
       </c>
       <c r="B27">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="C27">
-        <v>1.3699999999999999E-5</v>
+        <v>6.4599999999999998E-5</v>
       </c>
       <c r="D27">
         <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="33" t="s">
+      <c r="A28" t="s">
         <v>62</v>
       </c>
       <c r="B28">
-        <v>1158341</v>
+        <v>1158427</v>
       </c>
       <c r="C28">
-        <v>0.51238879999999998</v>
+        <v>0.51242690000000002</v>
       </c>
       <c r="D28">
         <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="33" t="s">
+      <c r="A29" t="s">
         <v>63</v>
       </c>
       <c r="B29">
-        <v>1901321</v>
+        <v>1901392</v>
       </c>
       <c r="C29">
-        <v>0.84104389999999996</v>
+        <v>0.84107529999999997</v>
       </c>
       <c r="D29">
         <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="33" t="s">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C30">
-        <v>4.8699999999999998E-5</v>
+        <v>7.1199999999999996E-5</v>
       </c>
       <c r="D30">
         <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="33" t="s">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
       <c r="B31">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C31">
-        <v>4.07E-5</v>
+        <v>5.9700000000000001E-5</v>
       </c>
       <c r="D31">
         <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="33" t="s">
+      <c r="A32" t="s">
         <v>64</v>
       </c>
       <c r="B32">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C32">
-        <v>2.3900000000000002E-5</v>
+        <v>4.07E-5</v>
       </c>
       <c r="D32">
         <v>102286</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="33" t="s">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33">
-        <v>1834</v>
+        <v>1862</v>
       </c>
       <c r="C33">
-        <v>8.1130000000000004E-4</v>
+        <v>8.2370000000000002E-4</v>
       </c>
       <c r="D33">
         <v>1540</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="33" t="s">
+      <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C34">
-        <v>2.2099999999999998E-5</v>
+        <v>3.2299999999999999E-5</v>
       </c>
       <c r="D34">
         <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="33" t="s">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
       <c r="B35">
@@ -6959,175 +6956,175 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="33" t="s">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="C36">
-        <v>7.5000000000000002E-6</v>
+        <v>3.9799999999999998E-5</v>
       </c>
       <c r="D36">
         <v>356239</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="33" t="s">
+      <c r="A37" t="s">
         <v>66</v>
       </c>
       <c r="B37">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="C37">
-        <v>9.3000000000000007E-6</v>
+        <v>3.54E-5</v>
       </c>
       <c r="D37">
         <v>368550</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="33" t="s">
+      <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C38">
-        <v>5.8000000000000004E-6</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="D38">
         <v>1633693</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="33" t="s">
+      <c r="A39" t="s">
         <v>67</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C39">
-        <v>4.8999999999999997E-6</v>
+        <v>1.77E-5</v>
       </c>
       <c r="D39">
         <v>1311060</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="33" t="s">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C40">
-        <v>3.9999999999999998E-6</v>
+        <v>1.59E-5</v>
       </c>
       <c r="D40">
         <v>486576</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="33" t="s">
+      <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C41">
-        <v>1.3E-6</v>
+        <v>7.5000000000000002E-6</v>
       </c>
       <c r="D41">
         <v>636000</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="33" t="s">
+      <c r="A42" t="s">
         <v>68</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C42">
-        <v>1.3E-6</v>
-      </c>
-      <c r="D42" s="34">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="D42" s="32">
         <v>18530</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="33" t="s">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43" s="34">
-        <v>8.9999999999999996E-7</v>
+        <v>19</v>
+      </c>
+      <c r="C43">
+        <v>8.3999999999999992E-6</v>
       </c>
       <c r="D43">
         <v>132850</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="33" t="s">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C44">
-        <v>2.7E-6</v>
+        <v>8.8000000000000004E-6</v>
       </c>
       <c r="D44">
         <v>146314</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="33" t="s">
+      <c r="A45" t="s">
         <v>69</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="C45">
-        <v>1.3E-6</v>
+        <v>3.01E-5</v>
       </c>
       <c r="D45">
         <v>704487</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="33" t="s">
+      <c r="A46" t="s">
         <v>70</v>
       </c>
       <c r="B46">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C46">
-        <v>1.9000000000000001E-5</v>
+        <v>5.66E-5</v>
       </c>
       <c r="D46">
         <v>223</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="33" t="s">
+      <c r="A47" t="s">
         <v>71</v>
       </c>
       <c r="B47">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="C47">
-        <v>1.5500000000000001E-5</v>
+        <v>4.5599999999999997E-5</v>
       </c>
       <c r="D47">
         <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="33" t="s">
+      <c r="A48" t="s">
         <v>74</v>
       </c>
       <c r="B48">
@@ -7141,7 +7138,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="33" t="s">
+      <c r="A49" t="s">
         <v>75</v>
       </c>
       <c r="B49">
@@ -7583,7 +7580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0259719E-8A60-4BBE-A5F9-5A66971B39D0}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>

</xml_diff>